<commit_message>
Update transportation variables to better represent properties of electric vs. ICE vehicles
</commit_message>
<xml_diff>
--- a/InputData/trans/BAADTbVT/BAU Avg Annual Dist Traveled by Veh Type.xlsx
+++ b/InputData/trans/BAADTbVT/BAU Avg Annual Dist Traveled by Veh Type.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us-analysis\InputData\trans\BAADTbVT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\trans\BAADTbVT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -43,7 +43,7 @@
     <definedName name="ti_tbl_69" localSheetId="8">#REF!</definedName>
     <definedName name="ti_tbl_69">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -4129,25 +4129,25 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="54" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="54" fillId="0" borderId="0" xfId="78" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="133" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="3" xfId="131" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="57" fillId="0" borderId="0" xfId="78" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="54" fillId="0" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="133" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="53" fillId="0" borderId="0" xfId="78" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="78" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="132" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="131" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="133" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="78" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -4169,20 +4169,20 @@
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="78" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="3" xfId="131" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="54" fillId="0" borderId="0" xfId="78" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="54" fillId="0" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="133" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="57" fillId="0" borderId="0" xfId="78" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="132" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="78" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="53" fillId="0" borderId="0" xfId="78" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="154">
@@ -5232,7 +5232,7 @@
   <dimension ref="A1:AH9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -5899,136 +5899,136 @@
         <v>9</v>
       </c>
       <c r="B6" s="15">
-        <f>SUM('NRBS 40'!D5,'NRBS 40'!D7,'NRBS 40'!D8)/SUM('NRBS 40'!B5,'NRBS 40'!B8,'NRBS 40'!B9)*1000</f>
-        <v>171.80862177031827</v>
+        <f>SUM('NRBS 40'!D5,'NRBS 40'!D7,'NRBS 40'!D8)/SUM('NRBS 40'!B5,'NRBS 40'!B7,'NRBS 40'!B8)*1000</f>
+        <v>194.17552144824873</v>
       </c>
       <c r="C6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="D6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="E6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="F6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="G6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="H6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="I6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="J6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="K6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="L6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="M6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="N6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="O6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="P6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="Q6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="R6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="S6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="T6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="U6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="V6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="W6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="X6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="Y6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="Z6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="AA6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="AB6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="AC6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="AD6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="AE6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="AF6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="AG6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
       <c r="AH6" s="15">
         <f t="shared" si="0"/>
-        <v>171.80862177031827</v>
+        <v>194.17552144824873</v>
       </c>
     </row>
     <row r="7" spans="1:34">
@@ -34936,41 +34936,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" s="37" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="69" t="s">
         <v>447</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="82"/>
-      <c r="U1" s="82"/>
-      <c r="V1" s="82"/>
-      <c r="W1" s="82"/>
-      <c r="X1" s="82"/>
-      <c r="Y1" s="82"/>
-      <c r="Z1" s="82"/>
-      <c r="AA1" s="82"/>
-      <c r="AB1" s="82"/>
-      <c r="AC1" s="82"/>
-      <c r="AD1" s="82"/>
-      <c r="AE1" s="82"/>
-      <c r="AF1" s="82"/>
-      <c r="AG1" s="82"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
+      <c r="Q1" s="69"/>
+      <c r="R1" s="69"/>
+      <c r="S1" s="69"/>
+      <c r="T1" s="69"/>
+      <c r="U1" s="69"/>
+      <c r="V1" s="69"/>
+      <c r="W1" s="69"/>
+      <c r="X1" s="69"/>
+      <c r="Y1" s="69"/>
+      <c r="Z1" s="69"/>
+      <c r="AA1" s="69"/>
+      <c r="AB1" s="69"/>
+      <c r="AC1" s="69"/>
+      <c r="AD1" s="69"/>
+      <c r="AE1" s="69"/>
+      <c r="AF1" s="69"/>
+      <c r="AG1" s="69"/>
       <c r="AI1" s="37" t="s">
         <v>448</v>
       </c>
@@ -37774,363 +37774,363 @@
       </c>
     </row>
     <row r="28" spans="1:36" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A28" s="83" t="s">
+      <c r="A28" s="70" t="s">
         <v>475</v>
       </c>
-      <c r="B28" s="83"/>
-      <c r="C28" s="83"/>
-      <c r="D28" s="83"/>
-      <c r="E28" s="83"/>
-      <c r="F28" s="83"/>
-      <c r="G28" s="83"/>
-      <c r="H28" s="83"/>
-      <c r="I28" s="83"/>
-      <c r="J28" s="83"/>
-      <c r="K28" s="83"/>
-      <c r="L28" s="83"/>
-      <c r="M28" s="83"/>
-      <c r="N28" s="83"/>
-      <c r="O28" s="83"/>
-      <c r="P28" s="83"/>
-      <c r="Q28" s="83"/>
-      <c r="R28" s="83"/>
-      <c r="S28" s="83"/>
-      <c r="T28" s="83"/>
-      <c r="U28" s="83"/>
-      <c r="V28" s="83"/>
-      <c r="W28" s="83"/>
-      <c r="X28" s="83"/>
-      <c r="Y28" s="83"/>
-      <c r="Z28" s="83"/>
+      <c r="B28" s="70"/>
+      <c r="C28" s="70"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="70"/>
+      <c r="G28" s="70"/>
+      <c r="H28" s="70"/>
+      <c r="I28" s="70"/>
+      <c r="J28" s="70"/>
+      <c r="K28" s="70"/>
+      <c r="L28" s="70"/>
+      <c r="M28" s="70"/>
+      <c r="N28" s="70"/>
+      <c r="O28" s="70"/>
+      <c r="P28" s="70"/>
+      <c r="Q28" s="70"/>
+      <c r="R28" s="70"/>
+      <c r="S28" s="70"/>
+      <c r="T28" s="70"/>
+      <c r="U28" s="70"/>
+      <c r="V28" s="70"/>
+      <c r="W28" s="70"/>
+      <c r="X28" s="70"/>
+      <c r="Y28" s="70"/>
+      <c r="Z28" s="70"/>
       <c r="AI28" s="47"/>
     </row>
     <row r="29" spans="1:36" s="42" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A29" s="84"/>
-      <c r="B29" s="84"/>
-      <c r="C29" s="84"/>
-      <c r="D29" s="84"/>
-      <c r="E29" s="84"/>
-      <c r="F29" s="84"/>
-      <c r="G29" s="84"/>
-      <c r="H29" s="84"/>
-      <c r="I29" s="84"/>
-      <c r="J29" s="84"/>
-      <c r="K29" s="84"/>
-      <c r="L29" s="84"/>
-      <c r="M29" s="84"/>
-      <c r="N29" s="84"/>
-      <c r="O29" s="84"/>
-      <c r="P29" s="84"/>
-      <c r="Q29" s="84"/>
-      <c r="R29" s="84"/>
-      <c r="S29" s="84"/>
-      <c r="T29" s="84"/>
-      <c r="U29" s="84"/>
-      <c r="V29" s="84"/>
-      <c r="W29" s="84"/>
-      <c r="X29" s="84"/>
-      <c r="Y29" s="84"/>
-      <c r="Z29" s="84"/>
+      <c r="A29" s="71"/>
+      <c r="B29" s="71"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="71"/>
+      <c r="E29" s="71"/>
+      <c r="F29" s="71"/>
+      <c r="G29" s="71"/>
+      <c r="H29" s="71"/>
+      <c r="I29" s="71"/>
+      <c r="J29" s="71"/>
+      <c r="K29" s="71"/>
+      <c r="L29" s="71"/>
+      <c r="M29" s="71"/>
+      <c r="N29" s="71"/>
+      <c r="O29" s="71"/>
+      <c r="P29" s="71"/>
+      <c r="Q29" s="71"/>
+      <c r="R29" s="71"/>
+      <c r="S29" s="71"/>
+      <c r="T29" s="71"/>
+      <c r="U29" s="71"/>
+      <c r="V29" s="71"/>
+      <c r="W29" s="71"/>
+      <c r="X29" s="71"/>
+      <c r="Y29" s="71"/>
+      <c r="Z29" s="71"/>
     </row>
     <row r="30" spans="1:36" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A30" s="85" t="s">
+      <c r="A30" s="72" t="s">
         <v>476</v>
       </c>
-      <c r="B30" s="85"/>
-      <c r="C30" s="85"/>
-      <c r="D30" s="85"/>
-      <c r="E30" s="85"/>
-      <c r="F30" s="85"/>
-      <c r="G30" s="85"/>
-      <c r="H30" s="85"/>
-      <c r="I30" s="85"/>
-      <c r="J30" s="85"/>
-      <c r="K30" s="85"/>
-      <c r="L30" s="85"/>
-      <c r="M30" s="85"/>
-      <c r="N30" s="85"/>
-      <c r="O30" s="85"/>
-      <c r="P30" s="85"/>
-      <c r="Q30" s="85"/>
-      <c r="R30" s="85"/>
-      <c r="S30" s="85"/>
-      <c r="T30" s="85"/>
-      <c r="U30" s="85"/>
-      <c r="V30" s="85"/>
-      <c r="W30" s="85"/>
-      <c r="X30" s="85"/>
-      <c r="Y30" s="85"/>
-      <c r="Z30" s="85"/>
+      <c r="B30" s="72"/>
+      <c r="C30" s="72"/>
+      <c r="D30" s="72"/>
+      <c r="E30" s="72"/>
+      <c r="F30" s="72"/>
+      <c r="G30" s="72"/>
+      <c r="H30" s="72"/>
+      <c r="I30" s="72"/>
+      <c r="J30" s="72"/>
+      <c r="K30" s="72"/>
+      <c r="L30" s="72"/>
+      <c r="M30" s="72"/>
+      <c r="N30" s="72"/>
+      <c r="O30" s="72"/>
+      <c r="P30" s="72"/>
+      <c r="Q30" s="72"/>
+      <c r="R30" s="72"/>
+      <c r="S30" s="72"/>
+      <c r="T30" s="72"/>
+      <c r="U30" s="72"/>
+      <c r="V30" s="72"/>
+      <c r="W30" s="72"/>
+      <c r="X30" s="72"/>
+      <c r="Y30" s="72"/>
+      <c r="Z30" s="72"/>
     </row>
     <row r="31" spans="1:36" s="64" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A31" s="85" t="s">
+      <c r="A31" s="72" t="s">
         <v>477</v>
       </c>
-      <c r="B31" s="85"/>
-      <c r="C31" s="85"/>
-      <c r="D31" s="85"/>
-      <c r="E31" s="85"/>
-      <c r="F31" s="85"/>
-      <c r="G31" s="85"/>
-      <c r="H31" s="85"/>
-      <c r="I31" s="85"/>
-      <c r="J31" s="85"/>
-      <c r="K31" s="85"/>
-      <c r="L31" s="85"/>
-      <c r="M31" s="85"/>
-      <c r="N31" s="85"/>
-      <c r="O31" s="85"/>
-      <c r="P31" s="85"/>
-      <c r="Q31" s="85"/>
-      <c r="R31" s="85"/>
-      <c r="S31" s="85"/>
-      <c r="T31" s="85"/>
-      <c r="U31" s="85"/>
-      <c r="V31" s="85"/>
-      <c r="W31" s="85"/>
-      <c r="X31" s="85"/>
-      <c r="Y31" s="85"/>
-      <c r="Z31" s="85"/>
+      <c r="B31" s="72"/>
+      <c r="C31" s="72"/>
+      <c r="D31" s="72"/>
+      <c r="E31" s="72"/>
+      <c r="F31" s="72"/>
+      <c r="G31" s="72"/>
+      <c r="H31" s="72"/>
+      <c r="I31" s="72"/>
+      <c r="J31" s="72"/>
+      <c r="K31" s="72"/>
+      <c r="L31" s="72"/>
+      <c r="M31" s="72"/>
+      <c r="N31" s="72"/>
+      <c r="O31" s="72"/>
+      <c r="P31" s="72"/>
+      <c r="Q31" s="72"/>
+      <c r="R31" s="72"/>
+      <c r="S31" s="72"/>
+      <c r="T31" s="72"/>
+      <c r="U31" s="72"/>
+      <c r="V31" s="72"/>
+      <c r="W31" s="72"/>
+      <c r="X31" s="72"/>
+      <c r="Y31" s="72"/>
+      <c r="Z31" s="72"/>
     </row>
     <row r="32" spans="1:36" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A32" s="74" t="s">
+      <c r="A32" s="68" t="s">
         <v>478</v>
       </c>
-      <c r="B32" s="74"/>
-      <c r="C32" s="74"/>
-      <c r="D32" s="74"/>
-      <c r="E32" s="74"/>
-      <c r="F32" s="74"/>
-      <c r="G32" s="74"/>
-      <c r="H32" s="74"/>
-      <c r="I32" s="74"/>
-      <c r="J32" s="74"/>
-      <c r="K32" s="74"/>
-      <c r="L32" s="74"/>
-      <c r="M32" s="74"/>
-      <c r="N32" s="74"/>
-      <c r="O32" s="74"/>
-      <c r="P32" s="74"/>
-      <c r="Q32" s="74"/>
-      <c r="R32" s="74"/>
-      <c r="S32" s="74"/>
-      <c r="T32" s="74"/>
-      <c r="U32" s="74"/>
-      <c r="V32" s="74"/>
-      <c r="W32" s="74"/>
-      <c r="X32" s="74"/>
-      <c r="Y32" s="74"/>
-      <c r="Z32" s="74"/>
+      <c r="B32" s="68"/>
+      <c r="C32" s="68"/>
+      <c r="D32" s="68"/>
+      <c r="E32" s="68"/>
+      <c r="F32" s="68"/>
+      <c r="G32" s="68"/>
+      <c r="H32" s="68"/>
+      <c r="I32" s="68"/>
+      <c r="J32" s="68"/>
+      <c r="K32" s="68"/>
+      <c r="L32" s="68"/>
+      <c r="M32" s="68"/>
+      <c r="N32" s="68"/>
+      <c r="O32" s="68"/>
+      <c r="P32" s="68"/>
+      <c r="Q32" s="68"/>
+      <c r="R32" s="68"/>
+      <c r="S32" s="68"/>
+      <c r="T32" s="68"/>
+      <c r="U32" s="68"/>
+      <c r="V32" s="68"/>
+      <c r="W32" s="68"/>
+      <c r="X32" s="68"/>
+      <c r="Y32" s="68"/>
+      <c r="Z32" s="68"/>
     </row>
     <row r="33" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A33" s="74" t="s">
+      <c r="A33" s="68" t="s">
         <v>479</v>
       </c>
-      <c r="B33" s="74"/>
-      <c r="C33" s="74"/>
-      <c r="D33" s="74"/>
-      <c r="E33" s="74"/>
-      <c r="F33" s="74"/>
-      <c r="G33" s="74"/>
-      <c r="H33" s="74"/>
-      <c r="I33" s="74"/>
-      <c r="J33" s="74"/>
-      <c r="K33" s="74"/>
-      <c r="L33" s="74"/>
-      <c r="M33" s="74"/>
-      <c r="N33" s="74"/>
-      <c r="O33" s="74"/>
-      <c r="P33" s="74"/>
-      <c r="Q33" s="74"/>
-      <c r="R33" s="74"/>
-      <c r="S33" s="74"/>
-      <c r="T33" s="74"/>
-      <c r="U33" s="74"/>
-      <c r="V33" s="74"/>
-      <c r="W33" s="74"/>
-      <c r="X33" s="74"/>
-      <c r="Y33" s="74"/>
-      <c r="Z33" s="74"/>
+      <c r="B33" s="68"/>
+      <c r="C33" s="68"/>
+      <c r="D33" s="68"/>
+      <c r="E33" s="68"/>
+      <c r="F33" s="68"/>
+      <c r="G33" s="68"/>
+      <c r="H33" s="68"/>
+      <c r="I33" s="68"/>
+      <c r="J33" s="68"/>
+      <c r="K33" s="68"/>
+      <c r="L33" s="68"/>
+      <c r="M33" s="68"/>
+      <c r="N33" s="68"/>
+      <c r="O33" s="68"/>
+      <c r="P33" s="68"/>
+      <c r="Q33" s="68"/>
+      <c r="R33" s="68"/>
+      <c r="S33" s="68"/>
+      <c r="T33" s="68"/>
+      <c r="U33" s="68"/>
+      <c r="V33" s="68"/>
+      <c r="W33" s="68"/>
+      <c r="X33" s="68"/>
+      <c r="Y33" s="68"/>
+      <c r="Z33" s="68"/>
     </row>
     <row r="34" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A34" s="74" t="s">
+      <c r="A34" s="68" t="s">
         <v>480</v>
       </c>
-      <c r="B34" s="74"/>
-      <c r="C34" s="74"/>
-      <c r="D34" s="74"/>
-      <c r="E34" s="74"/>
-      <c r="F34" s="74"/>
-      <c r="G34" s="74"/>
-      <c r="H34" s="74"/>
-      <c r="I34" s="74"/>
-      <c r="J34" s="74"/>
-      <c r="K34" s="74"/>
-      <c r="L34" s="74"/>
-      <c r="M34" s="74"/>
-      <c r="N34" s="74"/>
-      <c r="O34" s="74"/>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="74"/>
-      <c r="R34" s="74"/>
-      <c r="S34" s="74"/>
-      <c r="T34" s="74"/>
-      <c r="U34" s="74"/>
-      <c r="V34" s="74"/>
-      <c r="W34" s="74"/>
-      <c r="X34" s="74"/>
-      <c r="Y34" s="74"/>
-      <c r="Z34" s="74"/>
+      <c r="B34" s="68"/>
+      <c r="C34" s="68"/>
+      <c r="D34" s="68"/>
+      <c r="E34" s="68"/>
+      <c r="F34" s="68"/>
+      <c r="G34" s="68"/>
+      <c r="H34" s="68"/>
+      <c r="I34" s="68"/>
+      <c r="J34" s="68"/>
+      <c r="K34" s="68"/>
+      <c r="L34" s="68"/>
+      <c r="M34" s="68"/>
+      <c r="N34" s="68"/>
+      <c r="O34" s="68"/>
+      <c r="P34" s="68"/>
+      <c r="Q34" s="68"/>
+      <c r="R34" s="68"/>
+      <c r="S34" s="68"/>
+      <c r="T34" s="68"/>
+      <c r="U34" s="68"/>
+      <c r="V34" s="68"/>
+      <c r="W34" s="68"/>
+      <c r="X34" s="68"/>
+      <c r="Y34" s="68"/>
+      <c r="Z34" s="68"/>
     </row>
     <row r="35" spans="1:26" s="64" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A35" s="85" t="s">
+      <c r="A35" s="72" t="s">
         <v>481</v>
       </c>
-      <c r="B35" s="85"/>
-      <c r="C35" s="85"/>
-      <c r="D35" s="85"/>
-      <c r="E35" s="85"/>
-      <c r="F35" s="85"/>
-      <c r="G35" s="85"/>
-      <c r="H35" s="85"/>
-      <c r="I35" s="85"/>
-      <c r="J35" s="85"/>
-      <c r="K35" s="85"/>
-      <c r="L35" s="85"/>
-      <c r="M35" s="85"/>
-      <c r="N35" s="85"/>
-      <c r="O35" s="85"/>
-      <c r="P35" s="85"/>
-      <c r="Q35" s="85"/>
-      <c r="R35" s="85"/>
-      <c r="S35" s="85"/>
-      <c r="T35" s="85"/>
-      <c r="U35" s="85"/>
-      <c r="V35" s="85"/>
-      <c r="W35" s="85"/>
-      <c r="X35" s="85"/>
-      <c r="Y35" s="85"/>
-      <c r="Z35" s="85"/>
+      <c r="B35" s="72"/>
+      <c r="C35" s="72"/>
+      <c r="D35" s="72"/>
+      <c r="E35" s="72"/>
+      <c r="F35" s="72"/>
+      <c r="G35" s="72"/>
+      <c r="H35" s="72"/>
+      <c r="I35" s="72"/>
+      <c r="J35" s="72"/>
+      <c r="K35" s="72"/>
+      <c r="L35" s="72"/>
+      <c r="M35" s="72"/>
+      <c r="N35" s="72"/>
+      <c r="O35" s="72"/>
+      <c r="P35" s="72"/>
+      <c r="Q35" s="72"/>
+      <c r="R35" s="72"/>
+      <c r="S35" s="72"/>
+      <c r="T35" s="72"/>
+      <c r="U35" s="72"/>
+      <c r="V35" s="72"/>
+      <c r="W35" s="72"/>
+      <c r="X35" s="72"/>
+      <c r="Y35" s="72"/>
+      <c r="Z35" s="72"/>
     </row>
     <row r="36" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A36" s="86" t="s">
+      <c r="A36" s="73" t="s">
         <v>482</v>
       </c>
-      <c r="B36" s="86"/>
-      <c r="C36" s="86"/>
-      <c r="D36" s="86"/>
-      <c r="E36" s="86"/>
-      <c r="F36" s="86"/>
-      <c r="G36" s="86"/>
-      <c r="H36" s="86"/>
-      <c r="I36" s="86"/>
-      <c r="J36" s="86"/>
-      <c r="K36" s="86"/>
-      <c r="L36" s="86"/>
-      <c r="M36" s="86"/>
-      <c r="N36" s="86"/>
-      <c r="O36" s="86"/>
-      <c r="P36" s="86"/>
-      <c r="Q36" s="86"/>
-      <c r="R36" s="86"/>
-      <c r="S36" s="86"/>
-      <c r="T36" s="86"/>
-      <c r="U36" s="86"/>
-      <c r="V36" s="86"/>
-      <c r="W36" s="86"/>
-      <c r="X36" s="86"/>
-      <c r="Y36" s="86"/>
-      <c r="Z36" s="86"/>
+      <c r="B36" s="73"/>
+      <c r="C36" s="73"/>
+      <c r="D36" s="73"/>
+      <c r="E36" s="73"/>
+      <c r="F36" s="73"/>
+      <c r="G36" s="73"/>
+      <c r="H36" s="73"/>
+      <c r="I36" s="73"/>
+      <c r="J36" s="73"/>
+      <c r="K36" s="73"/>
+      <c r="L36" s="73"/>
+      <c r="M36" s="73"/>
+      <c r="N36" s="73"/>
+      <c r="O36" s="73"/>
+      <c r="P36" s="73"/>
+      <c r="Q36" s="73"/>
+      <c r="R36" s="73"/>
+      <c r="S36" s="73"/>
+      <c r="T36" s="73"/>
+      <c r="U36" s="73"/>
+      <c r="V36" s="73"/>
+      <c r="W36" s="73"/>
+      <c r="X36" s="73"/>
+      <c r="Y36" s="73"/>
+      <c r="Z36" s="73"/>
     </row>
     <row r="37" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A37" s="74" t="s">
+      <c r="A37" s="68" t="s">
         <v>483</v>
       </c>
-      <c r="B37" s="74"/>
-      <c r="C37" s="74"/>
-      <c r="D37" s="74"/>
-      <c r="E37" s="74"/>
-      <c r="F37" s="74"/>
-      <c r="G37" s="74"/>
-      <c r="H37" s="74"/>
-      <c r="I37" s="74"/>
-      <c r="J37" s="74"/>
-      <c r="K37" s="74"/>
-      <c r="L37" s="74"/>
-      <c r="M37" s="74"/>
-      <c r="N37" s="74"/>
-      <c r="O37" s="74"/>
-      <c r="P37" s="74"/>
-      <c r="Q37" s="74"/>
-      <c r="R37" s="74"/>
-      <c r="S37" s="74"/>
-      <c r="T37" s="74"/>
-      <c r="U37" s="74"/>
-      <c r="V37" s="74"/>
-      <c r="W37" s="74"/>
-      <c r="X37" s="74"/>
-      <c r="Y37" s="74"/>
-      <c r="Z37" s="74"/>
+      <c r="B37" s="68"/>
+      <c r="C37" s="68"/>
+      <c r="D37" s="68"/>
+      <c r="E37" s="68"/>
+      <c r="F37" s="68"/>
+      <c r="G37" s="68"/>
+      <c r="H37" s="68"/>
+      <c r="I37" s="68"/>
+      <c r="J37" s="68"/>
+      <c r="K37" s="68"/>
+      <c r="L37" s="68"/>
+      <c r="M37" s="68"/>
+      <c r="N37" s="68"/>
+      <c r="O37" s="68"/>
+      <c r="P37" s="68"/>
+      <c r="Q37" s="68"/>
+      <c r="R37" s="68"/>
+      <c r="S37" s="68"/>
+      <c r="T37" s="68"/>
+      <c r="U37" s="68"/>
+      <c r="V37" s="68"/>
+      <c r="W37" s="68"/>
+      <c r="X37" s="68"/>
+      <c r="Y37" s="68"/>
+      <c r="Z37" s="68"/>
     </row>
     <row r="38" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A38" s="74" t="s">
+      <c r="A38" s="68" t="s">
         <v>484</v>
       </c>
-      <c r="B38" s="74"/>
-      <c r="C38" s="74"/>
-      <c r="D38" s="74"/>
-      <c r="E38" s="74"/>
-      <c r="F38" s="74"/>
-      <c r="G38" s="74"/>
-      <c r="H38" s="74"/>
-      <c r="I38" s="74"/>
-      <c r="J38" s="74"/>
-      <c r="K38" s="74"/>
-      <c r="L38" s="74"/>
-      <c r="M38" s="74"/>
-      <c r="N38" s="74"/>
-      <c r="O38" s="74"/>
-      <c r="P38" s="74"/>
-      <c r="Q38" s="74"/>
-      <c r="R38" s="74"/>
-      <c r="S38" s="74"/>
-      <c r="T38" s="74"/>
-      <c r="U38" s="74"/>
-      <c r="V38" s="74"/>
-      <c r="W38" s="74"/>
-      <c r="X38" s="74"/>
-      <c r="Y38" s="74"/>
-      <c r="Z38" s="74"/>
+      <c r="B38" s="68"/>
+      <c r="C38" s="68"/>
+      <c r="D38" s="68"/>
+      <c r="E38" s="68"/>
+      <c r="F38" s="68"/>
+      <c r="G38" s="68"/>
+      <c r="H38" s="68"/>
+      <c r="I38" s="68"/>
+      <c r="J38" s="68"/>
+      <c r="K38" s="68"/>
+      <c r="L38" s="68"/>
+      <c r="M38" s="68"/>
+      <c r="N38" s="68"/>
+      <c r="O38" s="68"/>
+      <c r="P38" s="68"/>
+      <c r="Q38" s="68"/>
+      <c r="R38" s="68"/>
+      <c r="S38" s="68"/>
+      <c r="T38" s="68"/>
+      <c r="U38" s="68"/>
+      <c r="V38" s="68"/>
+      <c r="W38" s="68"/>
+      <c r="X38" s="68"/>
+      <c r="Y38" s="68"/>
+      <c r="Z38" s="68"/>
     </row>
     <row r="39" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A39" s="74" t="s">
+      <c r="A39" s="68" t="s">
         <v>485</v>
       </c>
-      <c r="B39" s="74"/>
-      <c r="C39" s="74"/>
-      <c r="D39" s="74"/>
-      <c r="E39" s="74"/>
-      <c r="F39" s="74"/>
-      <c r="G39" s="74"/>
-      <c r="H39" s="74"/>
-      <c r="I39" s="74"/>
-      <c r="J39" s="74"/>
-      <c r="K39" s="74"/>
-      <c r="L39" s="74"/>
-      <c r="M39" s="74"/>
-      <c r="N39" s="74"/>
-      <c r="O39" s="74"/>
-      <c r="P39" s="74"/>
-      <c r="Q39" s="74"/>
-      <c r="R39" s="74"/>
-      <c r="S39" s="74"/>
-      <c r="T39" s="74"/>
-      <c r="U39" s="74"/>
-      <c r="V39" s="74"/>
-      <c r="W39" s="74"/>
-      <c r="X39" s="74"/>
-      <c r="Y39" s="74"/>
-      <c r="Z39" s="74"/>
+      <c r="B39" s="68"/>
+      <c r="C39" s="68"/>
+      <c r="D39" s="68"/>
+      <c r="E39" s="68"/>
+      <c r="F39" s="68"/>
+      <c r="G39" s="68"/>
+      <c r="H39" s="68"/>
+      <c r="I39" s="68"/>
+      <c r="J39" s="68"/>
+      <c r="K39" s="68"/>
+      <c r="L39" s="68"/>
+      <c r="M39" s="68"/>
+      <c r="N39" s="68"/>
+      <c r="O39" s="68"/>
+      <c r="P39" s="68"/>
+      <c r="Q39" s="68"/>
+      <c r="R39" s="68"/>
+      <c r="S39" s="68"/>
+      <c r="T39" s="68"/>
+      <c r="U39" s="68"/>
+      <c r="V39" s="68"/>
+      <c r="W39" s="68"/>
+      <c r="X39" s="68"/>
+      <c r="Y39" s="68"/>
+      <c r="Z39" s="68"/>
     </row>
     <row r="40" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
       <c r="A40" s="75"/>
@@ -38399,1087 +38399,1133 @@
       <c r="Z48" s="81"/>
     </row>
     <row r="49" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A49" s="73" t="s">
+      <c r="A49" s="74" t="s">
         <v>493</v>
       </c>
-      <c r="B49" s="73"/>
-      <c r="C49" s="73"/>
-      <c r="D49" s="73"/>
-      <c r="E49" s="73"/>
-      <c r="F49" s="73"/>
-      <c r="G49" s="73"/>
-      <c r="H49" s="73"/>
-      <c r="I49" s="73"/>
-      <c r="J49" s="73"/>
-      <c r="K49" s="73"/>
-      <c r="L49" s="73"/>
-      <c r="M49" s="73"/>
-      <c r="N49" s="73"/>
-      <c r="O49" s="73"/>
-      <c r="P49" s="73"/>
-      <c r="Q49" s="73"/>
-      <c r="R49" s="73"/>
-      <c r="S49" s="73"/>
-      <c r="T49" s="73"/>
-      <c r="U49" s="73"/>
-      <c r="V49" s="73"/>
-      <c r="W49" s="73"/>
-      <c r="X49" s="73"/>
-      <c r="Y49" s="73"/>
-      <c r="Z49" s="73"/>
+      <c r="B49" s="74"/>
+      <c r="C49" s="74"/>
+      <c r="D49" s="74"/>
+      <c r="E49" s="74"/>
+      <c r="F49" s="74"/>
+      <c r="G49" s="74"/>
+      <c r="H49" s="74"/>
+      <c r="I49" s="74"/>
+      <c r="J49" s="74"/>
+      <c r="K49" s="74"/>
+      <c r="L49" s="74"/>
+      <c r="M49" s="74"/>
+      <c r="N49" s="74"/>
+      <c r="O49" s="74"/>
+      <c r="P49" s="74"/>
+      <c r="Q49" s="74"/>
+      <c r="R49" s="74"/>
+      <c r="S49" s="74"/>
+      <c r="T49" s="74"/>
+      <c r="U49" s="74"/>
+      <c r="V49" s="74"/>
+      <c r="W49" s="74"/>
+      <c r="X49" s="74"/>
+      <c r="Y49" s="74"/>
+      <c r="Z49" s="74"/>
     </row>
     <row r="50" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A50" s="73" t="s">
+      <c r="A50" s="74" t="s">
         <v>494</v>
       </c>
-      <c r="B50" s="73"/>
-      <c r="C50" s="73"/>
-      <c r="D50" s="73"/>
-      <c r="E50" s="73"/>
-      <c r="F50" s="73"/>
-      <c r="G50" s="73"/>
-      <c r="H50" s="73"/>
-      <c r="I50" s="73"/>
-      <c r="J50" s="73"/>
-      <c r="K50" s="73"/>
-      <c r="L50" s="73"/>
-      <c r="M50" s="73"/>
-      <c r="N50" s="73"/>
-      <c r="O50" s="73"/>
-      <c r="P50" s="73"/>
-      <c r="Q50" s="73"/>
-      <c r="R50" s="73"/>
-      <c r="S50" s="73"/>
-      <c r="T50" s="73"/>
-      <c r="U50" s="73"/>
-      <c r="V50" s="73"/>
-      <c r="W50" s="73"/>
-      <c r="X50" s="73"/>
-      <c r="Y50" s="73"/>
-      <c r="Z50" s="73"/>
+      <c r="B50" s="74"/>
+      <c r="C50" s="74"/>
+      <c r="D50" s="74"/>
+      <c r="E50" s="74"/>
+      <c r="F50" s="74"/>
+      <c r="G50" s="74"/>
+      <c r="H50" s="74"/>
+      <c r="I50" s="74"/>
+      <c r="J50" s="74"/>
+      <c r="K50" s="74"/>
+      <c r="L50" s="74"/>
+      <c r="M50" s="74"/>
+      <c r="N50" s="74"/>
+      <c r="O50" s="74"/>
+      <c r="P50" s="74"/>
+      <c r="Q50" s="74"/>
+      <c r="R50" s="74"/>
+      <c r="S50" s="74"/>
+      <c r="T50" s="74"/>
+      <c r="U50" s="74"/>
+      <c r="V50" s="74"/>
+      <c r="W50" s="74"/>
+      <c r="X50" s="74"/>
+      <c r="Y50" s="74"/>
+      <c r="Z50" s="74"/>
     </row>
     <row r="51" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A51" s="70" t="s">
+      <c r="A51" s="83" t="s">
         <v>495</v>
       </c>
-      <c r="B51" s="70"/>
-      <c r="C51" s="70"/>
-      <c r="D51" s="70"/>
-      <c r="E51" s="70"/>
-      <c r="F51" s="70"/>
-      <c r="G51" s="70"/>
-      <c r="H51" s="70"/>
-      <c r="I51" s="70"/>
-      <c r="J51" s="70"/>
-      <c r="K51" s="70"/>
-      <c r="L51" s="70"/>
-      <c r="M51" s="70"/>
-      <c r="N51" s="70"/>
-      <c r="O51" s="70"/>
-      <c r="P51" s="70"/>
-      <c r="Q51" s="70"/>
-      <c r="R51" s="70"/>
-      <c r="S51" s="70"/>
-      <c r="T51" s="70"/>
-      <c r="U51" s="70"/>
-      <c r="V51" s="70"/>
-      <c r="W51" s="70"/>
-      <c r="X51" s="70"/>
-      <c r="Y51" s="70"/>
-      <c r="Z51" s="70"/>
+      <c r="B51" s="83"/>
+      <c r="C51" s="83"/>
+      <c r="D51" s="83"/>
+      <c r="E51" s="83"/>
+      <c r="F51" s="83"/>
+      <c r="G51" s="83"/>
+      <c r="H51" s="83"/>
+      <c r="I51" s="83"/>
+      <c r="J51" s="83"/>
+      <c r="K51" s="83"/>
+      <c r="L51" s="83"/>
+      <c r="M51" s="83"/>
+      <c r="N51" s="83"/>
+      <c r="O51" s="83"/>
+      <c r="P51" s="83"/>
+      <c r="Q51" s="83"/>
+      <c r="R51" s="83"/>
+      <c r="S51" s="83"/>
+      <c r="T51" s="83"/>
+      <c r="U51" s="83"/>
+      <c r="V51" s="83"/>
+      <c r="W51" s="83"/>
+      <c r="X51" s="83"/>
+      <c r="Y51" s="83"/>
+      <c r="Z51" s="83"/>
     </row>
     <row r="52" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A52" s="68" t="s">
+      <c r="A52" s="82" t="s">
         <v>496</v>
       </c>
-      <c r="B52" s="68"/>
-      <c r="C52" s="68"/>
-      <c r="D52" s="68"/>
-      <c r="E52" s="68"/>
-      <c r="F52" s="68"/>
-      <c r="G52" s="68"/>
-      <c r="H52" s="68"/>
-      <c r="I52" s="68"/>
-      <c r="J52" s="68"/>
-      <c r="K52" s="68"/>
-      <c r="L52" s="68"/>
-      <c r="M52" s="68"/>
-      <c r="N52" s="68"/>
-      <c r="O52" s="68"/>
-      <c r="P52" s="68"/>
-      <c r="Q52" s="68"/>
-      <c r="R52" s="68"/>
-      <c r="S52" s="68"/>
-      <c r="T52" s="68"/>
-      <c r="U52" s="68"/>
-      <c r="V52" s="68"/>
-      <c r="W52" s="68"/>
-      <c r="X52" s="68"/>
-      <c r="Y52" s="68"/>
-      <c r="Z52" s="68"/>
+      <c r="B52" s="82"/>
+      <c r="C52" s="82"/>
+      <c r="D52" s="82"/>
+      <c r="E52" s="82"/>
+      <c r="F52" s="82"/>
+      <c r="G52" s="82"/>
+      <c r="H52" s="82"/>
+      <c r="I52" s="82"/>
+      <c r="J52" s="82"/>
+      <c r="K52" s="82"/>
+      <c r="L52" s="82"/>
+      <c r="M52" s="82"/>
+      <c r="N52" s="82"/>
+      <c r="O52" s="82"/>
+      <c r="P52" s="82"/>
+      <c r="Q52" s="82"/>
+      <c r="R52" s="82"/>
+      <c r="S52" s="82"/>
+      <c r="T52" s="82"/>
+      <c r="U52" s="82"/>
+      <c r="V52" s="82"/>
+      <c r="W52" s="82"/>
+      <c r="X52" s="82"/>
+      <c r="Y52" s="82"/>
+      <c r="Z52" s="82"/>
     </row>
     <row r="53" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A53" s="68" t="s">
+      <c r="A53" s="82" t="s">
         <v>497</v>
       </c>
-      <c r="B53" s="68"/>
-      <c r="C53" s="68"/>
-      <c r="D53" s="68"/>
-      <c r="E53" s="68"/>
-      <c r="F53" s="68"/>
-      <c r="G53" s="68"/>
-      <c r="H53" s="68"/>
-      <c r="I53" s="68"/>
-      <c r="J53" s="68"/>
-      <c r="K53" s="68"/>
-      <c r="L53" s="68"/>
-      <c r="M53" s="68"/>
-      <c r="N53" s="68"/>
-      <c r="O53" s="68"/>
-      <c r="P53" s="68"/>
-      <c r="Q53" s="68"/>
-      <c r="R53" s="68"/>
-      <c r="S53" s="68"/>
-      <c r="T53" s="68"/>
-      <c r="U53" s="68"/>
-      <c r="V53" s="68"/>
-      <c r="W53" s="68"/>
-      <c r="X53" s="68"/>
-      <c r="Y53" s="68"/>
-      <c r="Z53" s="68"/>
+      <c r="B53" s="82"/>
+      <c r="C53" s="82"/>
+      <c r="D53" s="82"/>
+      <c r="E53" s="82"/>
+      <c r="F53" s="82"/>
+      <c r="G53" s="82"/>
+      <c r="H53" s="82"/>
+      <c r="I53" s="82"/>
+      <c r="J53" s="82"/>
+      <c r="K53" s="82"/>
+      <c r="L53" s="82"/>
+      <c r="M53" s="82"/>
+      <c r="N53" s="82"/>
+      <c r="O53" s="82"/>
+      <c r="P53" s="82"/>
+      <c r="Q53" s="82"/>
+      <c r="R53" s="82"/>
+      <c r="S53" s="82"/>
+      <c r="T53" s="82"/>
+      <c r="U53" s="82"/>
+      <c r="V53" s="82"/>
+      <c r="W53" s="82"/>
+      <c r="X53" s="82"/>
+      <c r="Y53" s="82"/>
+      <c r="Z53" s="82"/>
     </row>
     <row r="54" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A54" s="72" t="s">
+      <c r="A54" s="84" t="s">
         <v>498</v>
       </c>
-      <c r="B54" s="72"/>
-      <c r="C54" s="72"/>
-      <c r="D54" s="72"/>
-      <c r="E54" s="72"/>
-      <c r="F54" s="72"/>
-      <c r="G54" s="72"/>
-      <c r="H54" s="72"/>
-      <c r="I54" s="72"/>
-      <c r="J54" s="72"/>
-      <c r="K54" s="72"/>
-      <c r="L54" s="72"/>
-      <c r="M54" s="72"/>
-      <c r="N54" s="72"/>
-      <c r="O54" s="72"/>
-      <c r="P54" s="72"/>
-      <c r="Q54" s="72"/>
-      <c r="R54" s="72"/>
-      <c r="S54" s="72"/>
-      <c r="T54" s="72"/>
-      <c r="U54" s="72"/>
-      <c r="V54" s="72"/>
-      <c r="W54" s="72"/>
-      <c r="X54" s="72"/>
-      <c r="Y54" s="72"/>
-      <c r="Z54" s="72"/>
+      <c r="B54" s="84"/>
+      <c r="C54" s="84"/>
+      <c r="D54" s="84"/>
+      <c r="E54" s="84"/>
+      <c r="F54" s="84"/>
+      <c r="G54" s="84"/>
+      <c r="H54" s="84"/>
+      <c r="I54" s="84"/>
+      <c r="J54" s="84"/>
+      <c r="K54" s="84"/>
+      <c r="L54" s="84"/>
+      <c r="M54" s="84"/>
+      <c r="N54" s="84"/>
+      <c r="O54" s="84"/>
+      <c r="P54" s="84"/>
+      <c r="Q54" s="84"/>
+      <c r="R54" s="84"/>
+      <c r="S54" s="84"/>
+      <c r="T54" s="84"/>
+      <c r="U54" s="84"/>
+      <c r="V54" s="84"/>
+      <c r="W54" s="84"/>
+      <c r="X54" s="84"/>
+      <c r="Y54" s="84"/>
+      <c r="Z54" s="84"/>
     </row>
     <row r="55" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A55" s="71" t="s">
+      <c r="A55" s="85" t="s">
         <v>499</v>
       </c>
-      <c r="B55" s="71"/>
-      <c r="C55" s="71"/>
-      <c r="D55" s="71"/>
-      <c r="E55" s="71"/>
-      <c r="F55" s="71"/>
-      <c r="G55" s="71"/>
-      <c r="H55" s="71"/>
-      <c r="I55" s="71"/>
-      <c r="J55" s="71"/>
-      <c r="K55" s="71"/>
-      <c r="L55" s="71"/>
-      <c r="M55" s="71"/>
-      <c r="N55" s="71"/>
-      <c r="O55" s="71"/>
-      <c r="P55" s="71"/>
-      <c r="Q55" s="71"/>
-      <c r="R55" s="71"/>
-      <c r="S55" s="71"/>
-      <c r="T55" s="71"/>
-      <c r="U55" s="71"/>
-      <c r="V55" s="71"/>
-      <c r="W55" s="71"/>
-      <c r="X55" s="71"/>
-      <c r="Y55" s="71"/>
-      <c r="Z55" s="71"/>
+      <c r="B55" s="85"/>
+      <c r="C55" s="85"/>
+      <c r="D55" s="85"/>
+      <c r="E55" s="85"/>
+      <c r="F55" s="85"/>
+      <c r="G55" s="85"/>
+      <c r="H55" s="85"/>
+      <c r="I55" s="85"/>
+      <c r="J55" s="85"/>
+      <c r="K55" s="85"/>
+      <c r="L55" s="85"/>
+      <c r="M55" s="85"/>
+      <c r="N55" s="85"/>
+      <c r="O55" s="85"/>
+      <c r="P55" s="85"/>
+      <c r="Q55" s="85"/>
+      <c r="R55" s="85"/>
+      <c r="S55" s="85"/>
+      <c r="T55" s="85"/>
+      <c r="U55" s="85"/>
+      <c r="V55" s="85"/>
+      <c r="W55" s="85"/>
+      <c r="X55" s="85"/>
+      <c r="Y55" s="85"/>
+      <c r="Z55" s="85"/>
     </row>
     <row r="56" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A56" s="70" t="s">
+      <c r="A56" s="83" t="s">
         <v>500</v>
       </c>
-      <c r="B56" s="70"/>
-      <c r="C56" s="70"/>
-      <c r="D56" s="70"/>
-      <c r="E56" s="70"/>
-      <c r="F56" s="70"/>
-      <c r="G56" s="70"/>
-      <c r="H56" s="70"/>
-      <c r="I56" s="70"/>
-      <c r="J56" s="70"/>
-      <c r="K56" s="70"/>
-      <c r="L56" s="70"/>
-      <c r="M56" s="70"/>
-      <c r="N56" s="70"/>
-      <c r="O56" s="70"/>
-      <c r="P56" s="70"/>
-      <c r="Q56" s="70"/>
-      <c r="R56" s="70"/>
-      <c r="S56" s="70"/>
-      <c r="T56" s="70"/>
-      <c r="U56" s="70"/>
-      <c r="V56" s="70"/>
-      <c r="W56" s="70"/>
-      <c r="X56" s="70"/>
-      <c r="Y56" s="70"/>
-      <c r="Z56" s="70"/>
+      <c r="B56" s="83"/>
+      <c r="C56" s="83"/>
+      <c r="D56" s="83"/>
+      <c r="E56" s="83"/>
+      <c r="F56" s="83"/>
+      <c r="G56" s="83"/>
+      <c r="H56" s="83"/>
+      <c r="I56" s="83"/>
+      <c r="J56" s="83"/>
+      <c r="K56" s="83"/>
+      <c r="L56" s="83"/>
+      <c r="M56" s="83"/>
+      <c r="N56" s="83"/>
+      <c r="O56" s="83"/>
+      <c r="P56" s="83"/>
+      <c r="Q56" s="83"/>
+      <c r="R56" s="83"/>
+      <c r="S56" s="83"/>
+      <c r="T56" s="83"/>
+      <c r="U56" s="83"/>
+      <c r="V56" s="83"/>
+      <c r="W56" s="83"/>
+      <c r="X56" s="83"/>
+      <c r="Y56" s="83"/>
+      <c r="Z56" s="83"/>
     </row>
     <row r="57" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A57" s="72" t="s">
+      <c r="A57" s="84" t="s">
         <v>501</v>
       </c>
-      <c r="B57" s="72"/>
-      <c r="C57" s="72"/>
-      <c r="D57" s="72"/>
-      <c r="E57" s="72"/>
-      <c r="F57" s="72"/>
-      <c r="G57" s="72"/>
-      <c r="H57" s="72"/>
-      <c r="I57" s="72"/>
-      <c r="J57" s="72"/>
-      <c r="K57" s="72"/>
-      <c r="L57" s="72"/>
-      <c r="M57" s="72"/>
-      <c r="N57" s="72"/>
-      <c r="O57" s="72"/>
-      <c r="P57" s="72"/>
-      <c r="Q57" s="72"/>
-      <c r="R57" s="72"/>
-      <c r="S57" s="72"/>
-      <c r="T57" s="72"/>
-      <c r="U57" s="72"/>
-      <c r="V57" s="72"/>
-      <c r="W57" s="72"/>
-      <c r="X57" s="72"/>
-      <c r="Y57" s="72"/>
-      <c r="Z57" s="72"/>
+      <c r="B57" s="84"/>
+      <c r="C57" s="84"/>
+      <c r="D57" s="84"/>
+      <c r="E57" s="84"/>
+      <c r="F57" s="84"/>
+      <c r="G57" s="84"/>
+      <c r="H57" s="84"/>
+      <c r="I57" s="84"/>
+      <c r="J57" s="84"/>
+      <c r="K57" s="84"/>
+      <c r="L57" s="84"/>
+      <c r="M57" s="84"/>
+      <c r="N57" s="84"/>
+      <c r="O57" s="84"/>
+      <c r="P57" s="84"/>
+      <c r="Q57" s="84"/>
+      <c r="R57" s="84"/>
+      <c r="S57" s="84"/>
+      <c r="T57" s="84"/>
+      <c r="U57" s="84"/>
+      <c r="V57" s="84"/>
+      <c r="W57" s="84"/>
+      <c r="X57" s="84"/>
+      <c r="Y57" s="84"/>
+      <c r="Z57" s="84"/>
     </row>
     <row r="58" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A58" s="68" t="s">
+      <c r="A58" s="82" t="s">
         <v>502</v>
       </c>
-      <c r="B58" s="68"/>
-      <c r="C58" s="68"/>
-      <c r="D58" s="68"/>
-      <c r="E58" s="68"/>
-      <c r="F58" s="68"/>
-      <c r="G58" s="68"/>
-      <c r="H58" s="68"/>
-      <c r="I58" s="68"/>
-      <c r="J58" s="68"/>
-      <c r="K58" s="68"/>
-      <c r="L58" s="68"/>
-      <c r="M58" s="68"/>
-      <c r="N58" s="68"/>
-      <c r="O58" s="68"/>
-      <c r="P58" s="68"/>
-      <c r="Q58" s="68"/>
-      <c r="R58" s="68"/>
-      <c r="S58" s="68"/>
-      <c r="T58" s="68"/>
-      <c r="U58" s="68"/>
-      <c r="V58" s="68"/>
-      <c r="W58" s="68"/>
-      <c r="X58" s="68"/>
-      <c r="Y58" s="68"/>
-      <c r="Z58" s="68"/>
+      <c r="B58" s="82"/>
+      <c r="C58" s="82"/>
+      <c r="D58" s="82"/>
+      <c r="E58" s="82"/>
+      <c r="F58" s="82"/>
+      <c r="G58" s="82"/>
+      <c r="H58" s="82"/>
+      <c r="I58" s="82"/>
+      <c r="J58" s="82"/>
+      <c r="K58" s="82"/>
+      <c r="L58" s="82"/>
+      <c r="M58" s="82"/>
+      <c r="N58" s="82"/>
+      <c r="O58" s="82"/>
+      <c r="P58" s="82"/>
+      <c r="Q58" s="82"/>
+      <c r="R58" s="82"/>
+      <c r="S58" s="82"/>
+      <c r="T58" s="82"/>
+      <c r="U58" s="82"/>
+      <c r="V58" s="82"/>
+      <c r="W58" s="82"/>
+      <c r="X58" s="82"/>
+      <c r="Y58" s="82"/>
+      <c r="Z58" s="82"/>
     </row>
     <row r="59" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A59" s="70" t="s">
+      <c r="A59" s="83" t="s">
         <v>503</v>
       </c>
-      <c r="B59" s="70"/>
-      <c r="C59" s="70"/>
-      <c r="D59" s="70"/>
-      <c r="E59" s="70"/>
-      <c r="F59" s="70"/>
-      <c r="G59" s="70"/>
-      <c r="H59" s="70"/>
-      <c r="I59" s="70"/>
-      <c r="J59" s="70"/>
-      <c r="K59" s="70"/>
-      <c r="L59" s="70"/>
-      <c r="M59" s="70"/>
-      <c r="N59" s="70"/>
-      <c r="O59" s="70"/>
-      <c r="P59" s="70"/>
-      <c r="Q59" s="70"/>
-      <c r="R59" s="70"/>
-      <c r="S59" s="70"/>
-      <c r="T59" s="70"/>
-      <c r="U59" s="70"/>
-      <c r="V59" s="70"/>
-      <c r="W59" s="70"/>
-      <c r="X59" s="70"/>
-      <c r="Y59" s="70"/>
-      <c r="Z59" s="70"/>
+      <c r="B59" s="83"/>
+      <c r="C59" s="83"/>
+      <c r="D59" s="83"/>
+      <c r="E59" s="83"/>
+      <c r="F59" s="83"/>
+      <c r="G59" s="83"/>
+      <c r="H59" s="83"/>
+      <c r="I59" s="83"/>
+      <c r="J59" s="83"/>
+      <c r="K59" s="83"/>
+      <c r="L59" s="83"/>
+      <c r="M59" s="83"/>
+      <c r="N59" s="83"/>
+      <c r="O59" s="83"/>
+      <c r="P59" s="83"/>
+      <c r="Q59" s="83"/>
+      <c r="R59" s="83"/>
+      <c r="S59" s="83"/>
+      <c r="T59" s="83"/>
+      <c r="U59" s="83"/>
+      <c r="V59" s="83"/>
+      <c r="W59" s="83"/>
+      <c r="X59" s="83"/>
+      <c r="Y59" s="83"/>
+      <c r="Z59" s="83"/>
     </row>
     <row r="60" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A60" s="68" t="s">
+      <c r="A60" s="82" t="s">
         <v>504</v>
       </c>
-      <c r="B60" s="68"/>
-      <c r="C60" s="68"/>
-      <c r="D60" s="68"/>
-      <c r="E60" s="68"/>
-      <c r="F60" s="68"/>
-      <c r="G60" s="68"/>
-      <c r="H60" s="68"/>
-      <c r="I60" s="68"/>
-      <c r="J60" s="68"/>
-      <c r="K60" s="68"/>
-      <c r="L60" s="68"/>
-      <c r="M60" s="68"/>
-      <c r="N60" s="68"/>
-      <c r="O60" s="68"/>
-      <c r="P60" s="68"/>
-      <c r="Q60" s="68"/>
-      <c r="R60" s="68"/>
-      <c r="S60" s="68"/>
-      <c r="T60" s="68"/>
-      <c r="U60" s="68"/>
-      <c r="V60" s="68"/>
-      <c r="W60" s="68"/>
-      <c r="X60" s="68"/>
-      <c r="Y60" s="68"/>
-      <c r="Z60" s="68"/>
+      <c r="B60" s="82"/>
+      <c r="C60" s="82"/>
+      <c r="D60" s="82"/>
+      <c r="E60" s="82"/>
+      <c r="F60" s="82"/>
+      <c r="G60" s="82"/>
+      <c r="H60" s="82"/>
+      <c r="I60" s="82"/>
+      <c r="J60" s="82"/>
+      <c r="K60" s="82"/>
+      <c r="L60" s="82"/>
+      <c r="M60" s="82"/>
+      <c r="N60" s="82"/>
+      <c r="O60" s="82"/>
+      <c r="P60" s="82"/>
+      <c r="Q60" s="82"/>
+      <c r="R60" s="82"/>
+      <c r="S60" s="82"/>
+      <c r="T60" s="82"/>
+      <c r="U60" s="82"/>
+      <c r="V60" s="82"/>
+      <c r="W60" s="82"/>
+      <c r="X60" s="82"/>
+      <c r="Y60" s="82"/>
+      <c r="Z60" s="82"/>
     </row>
     <row r="61" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A61" s="70" t="s">
+      <c r="A61" s="83" t="s">
         <v>505</v>
       </c>
-      <c r="B61" s="70"/>
-      <c r="C61" s="70"/>
-      <c r="D61" s="70"/>
-      <c r="E61" s="70"/>
-      <c r="F61" s="70"/>
-      <c r="G61" s="70"/>
-      <c r="H61" s="70"/>
-      <c r="I61" s="70"/>
-      <c r="J61" s="70"/>
-      <c r="K61" s="70"/>
-      <c r="L61" s="70"/>
-      <c r="M61" s="70"/>
-      <c r="N61" s="70"/>
-      <c r="O61" s="70"/>
-      <c r="P61" s="70"/>
-      <c r="Q61" s="70"/>
-      <c r="R61" s="70"/>
-      <c r="S61" s="70"/>
-      <c r="T61" s="70"/>
-      <c r="U61" s="70"/>
-      <c r="V61" s="70"/>
-      <c r="W61" s="70"/>
-      <c r="X61" s="70"/>
-      <c r="Y61" s="70"/>
-      <c r="Z61" s="70"/>
+      <c r="B61" s="83"/>
+      <c r="C61" s="83"/>
+      <c r="D61" s="83"/>
+      <c r="E61" s="83"/>
+      <c r="F61" s="83"/>
+      <c r="G61" s="83"/>
+      <c r="H61" s="83"/>
+      <c r="I61" s="83"/>
+      <c r="J61" s="83"/>
+      <c r="K61" s="83"/>
+      <c r="L61" s="83"/>
+      <c r="M61" s="83"/>
+      <c r="N61" s="83"/>
+      <c r="O61" s="83"/>
+      <c r="P61" s="83"/>
+      <c r="Q61" s="83"/>
+      <c r="R61" s="83"/>
+      <c r="S61" s="83"/>
+      <c r="T61" s="83"/>
+      <c r="U61" s="83"/>
+      <c r="V61" s="83"/>
+      <c r="W61" s="83"/>
+      <c r="X61" s="83"/>
+      <c r="Y61" s="83"/>
+      <c r="Z61" s="83"/>
     </row>
     <row r="62" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A62" s="68" t="s">
+      <c r="A62" s="82" t="s">
         <v>506</v>
       </c>
-      <c r="B62" s="68"/>
-      <c r="C62" s="68"/>
-      <c r="D62" s="68"/>
-      <c r="E62" s="68"/>
-      <c r="F62" s="68"/>
-      <c r="G62" s="68"/>
-      <c r="H62" s="68"/>
-      <c r="I62" s="68"/>
-      <c r="J62" s="68"/>
-      <c r="K62" s="68"/>
-      <c r="L62" s="68"/>
-      <c r="M62" s="68"/>
-      <c r="N62" s="68"/>
-      <c r="O62" s="68"/>
-      <c r="P62" s="68"/>
-      <c r="Q62" s="68"/>
-      <c r="R62" s="68"/>
-      <c r="S62" s="68"/>
-      <c r="T62" s="68"/>
-      <c r="U62" s="68"/>
-      <c r="V62" s="68"/>
-      <c r="W62" s="68"/>
-      <c r="X62" s="68"/>
-      <c r="Y62" s="68"/>
-      <c r="Z62" s="68"/>
+      <c r="B62" s="82"/>
+      <c r="C62" s="82"/>
+      <c r="D62" s="82"/>
+      <c r="E62" s="82"/>
+      <c r="F62" s="82"/>
+      <c r="G62" s="82"/>
+      <c r="H62" s="82"/>
+      <c r="I62" s="82"/>
+      <c r="J62" s="82"/>
+      <c r="K62" s="82"/>
+      <c r="L62" s="82"/>
+      <c r="M62" s="82"/>
+      <c r="N62" s="82"/>
+      <c r="O62" s="82"/>
+      <c r="P62" s="82"/>
+      <c r="Q62" s="82"/>
+      <c r="R62" s="82"/>
+      <c r="S62" s="82"/>
+      <c r="T62" s="82"/>
+      <c r="U62" s="82"/>
+      <c r="V62" s="82"/>
+      <c r="W62" s="82"/>
+      <c r="X62" s="82"/>
+      <c r="Y62" s="82"/>
+      <c r="Z62" s="82"/>
     </row>
     <row r="63" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A63" s="68" t="s">
+      <c r="A63" s="82" t="s">
         <v>507</v>
       </c>
-      <c r="B63" s="68"/>
-      <c r="C63" s="68"/>
-      <c r="D63" s="68"/>
-      <c r="E63" s="68"/>
-      <c r="F63" s="68"/>
-      <c r="G63" s="68"/>
-      <c r="H63" s="68"/>
-      <c r="I63" s="68"/>
-      <c r="J63" s="68"/>
-      <c r="K63" s="68"/>
-      <c r="L63" s="68"/>
-      <c r="M63" s="68"/>
-      <c r="N63" s="68"/>
-      <c r="O63" s="68"/>
-      <c r="P63" s="68"/>
-      <c r="Q63" s="68"/>
-      <c r="R63" s="68"/>
-      <c r="S63" s="68"/>
-      <c r="T63" s="68"/>
-      <c r="U63" s="68"/>
-      <c r="V63" s="68"/>
-      <c r="W63" s="68"/>
-      <c r="X63" s="68"/>
-      <c r="Y63" s="68"/>
-      <c r="Z63" s="68"/>
+      <c r="B63" s="82"/>
+      <c r="C63" s="82"/>
+      <c r="D63" s="82"/>
+      <c r="E63" s="82"/>
+      <c r="F63" s="82"/>
+      <c r="G63" s="82"/>
+      <c r="H63" s="82"/>
+      <c r="I63" s="82"/>
+      <c r="J63" s="82"/>
+      <c r="K63" s="82"/>
+      <c r="L63" s="82"/>
+      <c r="M63" s="82"/>
+      <c r="N63" s="82"/>
+      <c r="O63" s="82"/>
+      <c r="P63" s="82"/>
+      <c r="Q63" s="82"/>
+      <c r="R63" s="82"/>
+      <c r="S63" s="82"/>
+      <c r="T63" s="82"/>
+      <c r="U63" s="82"/>
+      <c r="V63" s="82"/>
+      <c r="W63" s="82"/>
+      <c r="X63" s="82"/>
+      <c r="Y63" s="82"/>
+      <c r="Z63" s="82"/>
     </row>
     <row r="64" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A64" s="70" t="s">
+      <c r="A64" s="83" t="s">
         <v>508</v>
       </c>
-      <c r="B64" s="70"/>
-      <c r="C64" s="70"/>
-      <c r="D64" s="70"/>
-      <c r="E64" s="70"/>
-      <c r="F64" s="70"/>
-      <c r="G64" s="70"/>
-      <c r="H64" s="70"/>
-      <c r="I64" s="70"/>
-      <c r="J64" s="70"/>
-      <c r="K64" s="70"/>
-      <c r="L64" s="70"/>
-      <c r="M64" s="70"/>
-      <c r="N64" s="70"/>
-      <c r="O64" s="70"/>
-      <c r="P64" s="70"/>
-      <c r="Q64" s="70"/>
-      <c r="R64" s="70"/>
-      <c r="S64" s="70"/>
-      <c r="T64" s="70"/>
-      <c r="U64" s="70"/>
-      <c r="V64" s="70"/>
-      <c r="W64" s="70"/>
-      <c r="X64" s="70"/>
-      <c r="Y64" s="70"/>
-      <c r="Z64" s="70"/>
+      <c r="B64" s="83"/>
+      <c r="C64" s="83"/>
+      <c r="D64" s="83"/>
+      <c r="E64" s="83"/>
+      <c r="F64" s="83"/>
+      <c r="G64" s="83"/>
+      <c r="H64" s="83"/>
+      <c r="I64" s="83"/>
+      <c r="J64" s="83"/>
+      <c r="K64" s="83"/>
+      <c r="L64" s="83"/>
+      <c r="M64" s="83"/>
+      <c r="N64" s="83"/>
+      <c r="O64" s="83"/>
+      <c r="P64" s="83"/>
+      <c r="Q64" s="83"/>
+      <c r="R64" s="83"/>
+      <c r="S64" s="83"/>
+      <c r="T64" s="83"/>
+      <c r="U64" s="83"/>
+      <c r="V64" s="83"/>
+      <c r="W64" s="83"/>
+      <c r="X64" s="83"/>
+      <c r="Y64" s="83"/>
+      <c r="Z64" s="83"/>
     </row>
     <row r="65" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A65" s="72" t="s">
+      <c r="A65" s="84" t="s">
         <v>509</v>
       </c>
-      <c r="B65" s="72"/>
-      <c r="C65" s="72"/>
-      <c r="D65" s="72"/>
-      <c r="E65" s="72"/>
-      <c r="F65" s="72"/>
-      <c r="G65" s="72"/>
-      <c r="H65" s="72"/>
-      <c r="I65" s="72"/>
-      <c r="J65" s="72"/>
-      <c r="K65" s="72"/>
-      <c r="L65" s="72"/>
-      <c r="M65" s="72"/>
-      <c r="N65" s="72"/>
-      <c r="O65" s="72"/>
-      <c r="P65" s="72"/>
-      <c r="Q65" s="72"/>
-      <c r="R65" s="72"/>
-      <c r="S65" s="72"/>
-      <c r="T65" s="72"/>
-      <c r="U65" s="72"/>
-      <c r="V65" s="72"/>
-      <c r="W65" s="72"/>
-      <c r="X65" s="72"/>
-      <c r="Y65" s="72"/>
-      <c r="Z65" s="72"/>
+      <c r="B65" s="84"/>
+      <c r="C65" s="84"/>
+      <c r="D65" s="84"/>
+      <c r="E65" s="84"/>
+      <c r="F65" s="84"/>
+      <c r="G65" s="84"/>
+      <c r="H65" s="84"/>
+      <c r="I65" s="84"/>
+      <c r="J65" s="84"/>
+      <c r="K65" s="84"/>
+      <c r="L65" s="84"/>
+      <c r="M65" s="84"/>
+      <c r="N65" s="84"/>
+      <c r="O65" s="84"/>
+      <c r="P65" s="84"/>
+      <c r="Q65" s="84"/>
+      <c r="R65" s="84"/>
+      <c r="S65" s="84"/>
+      <c r="T65" s="84"/>
+      <c r="U65" s="84"/>
+      <c r="V65" s="84"/>
+      <c r="W65" s="84"/>
+      <c r="X65" s="84"/>
+      <c r="Y65" s="84"/>
+      <c r="Z65" s="84"/>
     </row>
     <row r="66" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A66" s="68" t="s">
+      <c r="A66" s="82" t="s">
         <v>502</v>
       </c>
-      <c r="B66" s="68"/>
-      <c r="C66" s="68"/>
-      <c r="D66" s="68"/>
-      <c r="E66" s="68"/>
-      <c r="F66" s="68"/>
-      <c r="G66" s="68"/>
-      <c r="H66" s="68"/>
-      <c r="I66" s="68"/>
-      <c r="J66" s="68"/>
-      <c r="K66" s="68"/>
-      <c r="L66" s="68"/>
-      <c r="M66" s="68"/>
-      <c r="N66" s="68"/>
-      <c r="O66" s="68"/>
-      <c r="P66" s="68"/>
-      <c r="Q66" s="68"/>
-      <c r="R66" s="68"/>
-      <c r="S66" s="68"/>
-      <c r="T66" s="68"/>
-      <c r="U66" s="68"/>
-      <c r="V66" s="68"/>
-      <c r="W66" s="68"/>
-      <c r="X66" s="68"/>
-      <c r="Y66" s="68"/>
-      <c r="Z66" s="68"/>
+      <c r="B66" s="82"/>
+      <c r="C66" s="82"/>
+      <c r="D66" s="82"/>
+      <c r="E66" s="82"/>
+      <c r="F66" s="82"/>
+      <c r="G66" s="82"/>
+      <c r="H66" s="82"/>
+      <c r="I66" s="82"/>
+      <c r="J66" s="82"/>
+      <c r="K66" s="82"/>
+      <c r="L66" s="82"/>
+      <c r="M66" s="82"/>
+      <c r="N66" s="82"/>
+      <c r="O66" s="82"/>
+      <c r="P66" s="82"/>
+      <c r="Q66" s="82"/>
+      <c r="R66" s="82"/>
+      <c r="S66" s="82"/>
+      <c r="T66" s="82"/>
+      <c r="U66" s="82"/>
+      <c r="V66" s="82"/>
+      <c r="W66" s="82"/>
+      <c r="X66" s="82"/>
+      <c r="Y66" s="82"/>
+      <c r="Z66" s="82"/>
     </row>
     <row r="67" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A67" s="70" t="s">
+      <c r="A67" s="83" t="s">
         <v>510</v>
       </c>
-      <c r="B67" s="70"/>
-      <c r="C67" s="70"/>
-      <c r="D67" s="70"/>
-      <c r="E67" s="70"/>
-      <c r="F67" s="70"/>
-      <c r="G67" s="70"/>
-      <c r="H67" s="70"/>
-      <c r="I67" s="70"/>
-      <c r="J67" s="70"/>
-      <c r="K67" s="70"/>
-      <c r="L67" s="70"/>
-      <c r="M67" s="70"/>
-      <c r="N67" s="70"/>
-      <c r="O67" s="70"/>
-      <c r="P67" s="70"/>
-      <c r="Q67" s="70"/>
-      <c r="R67" s="70"/>
-      <c r="S67" s="70"/>
-      <c r="T67" s="70"/>
-      <c r="U67" s="70"/>
-      <c r="V67" s="70"/>
-      <c r="W67" s="70"/>
-      <c r="X67" s="70"/>
-      <c r="Y67" s="70"/>
-      <c r="Z67" s="70"/>
+      <c r="B67" s="83"/>
+      <c r="C67" s="83"/>
+      <c r="D67" s="83"/>
+      <c r="E67" s="83"/>
+      <c r="F67" s="83"/>
+      <c r="G67" s="83"/>
+      <c r="H67" s="83"/>
+      <c r="I67" s="83"/>
+      <c r="J67" s="83"/>
+      <c r="K67" s="83"/>
+      <c r="L67" s="83"/>
+      <c r="M67" s="83"/>
+      <c r="N67" s="83"/>
+      <c r="O67" s="83"/>
+      <c r="P67" s="83"/>
+      <c r="Q67" s="83"/>
+      <c r="R67" s="83"/>
+      <c r="S67" s="83"/>
+      <c r="T67" s="83"/>
+      <c r="U67" s="83"/>
+      <c r="V67" s="83"/>
+      <c r="W67" s="83"/>
+      <c r="X67" s="83"/>
+      <c r="Y67" s="83"/>
+      <c r="Z67" s="83"/>
     </row>
     <row r="68" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A68" s="68" t="s">
+      <c r="A68" s="82" t="s">
         <v>511</v>
       </c>
-      <c r="B68" s="68"/>
-      <c r="C68" s="68"/>
-      <c r="D68" s="68"/>
-      <c r="E68" s="68"/>
-      <c r="F68" s="68"/>
-      <c r="G68" s="68"/>
-      <c r="H68" s="68"/>
-      <c r="I68" s="68"/>
-      <c r="J68" s="68"/>
-      <c r="K68" s="68"/>
-      <c r="L68" s="68"/>
-      <c r="M68" s="68"/>
-      <c r="N68" s="68"/>
-      <c r="O68" s="68"/>
-      <c r="P68" s="68"/>
-      <c r="Q68" s="68"/>
-      <c r="R68" s="68"/>
-      <c r="S68" s="68"/>
-      <c r="T68" s="68"/>
-      <c r="U68" s="68"/>
-      <c r="V68" s="68"/>
-      <c r="W68" s="68"/>
-      <c r="X68" s="68"/>
-      <c r="Y68" s="68"/>
-      <c r="Z68" s="68"/>
+      <c r="B68" s="82"/>
+      <c r="C68" s="82"/>
+      <c r="D68" s="82"/>
+      <c r="E68" s="82"/>
+      <c r="F68" s="82"/>
+      <c r="G68" s="82"/>
+      <c r="H68" s="82"/>
+      <c r="I68" s="82"/>
+      <c r="J68" s="82"/>
+      <c r="K68" s="82"/>
+      <c r="L68" s="82"/>
+      <c r="M68" s="82"/>
+      <c r="N68" s="82"/>
+      <c r="O68" s="82"/>
+      <c r="P68" s="82"/>
+      <c r="Q68" s="82"/>
+      <c r="R68" s="82"/>
+      <c r="S68" s="82"/>
+      <c r="T68" s="82"/>
+      <c r="U68" s="82"/>
+      <c r="V68" s="82"/>
+      <c r="W68" s="82"/>
+      <c r="X68" s="82"/>
+      <c r="Y68" s="82"/>
+      <c r="Z68" s="82"/>
     </row>
     <row r="69" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A69" s="70" t="s">
+      <c r="A69" s="83" t="s">
         <v>512</v>
       </c>
-      <c r="B69" s="70"/>
-      <c r="C69" s="70"/>
-      <c r="D69" s="70"/>
-      <c r="E69" s="70"/>
-      <c r="F69" s="70"/>
-      <c r="G69" s="70"/>
-      <c r="H69" s="70"/>
-      <c r="I69" s="70"/>
-      <c r="J69" s="70"/>
-      <c r="K69" s="70"/>
-      <c r="L69" s="70"/>
-      <c r="M69" s="70"/>
-      <c r="N69" s="70"/>
-      <c r="O69" s="70"/>
-      <c r="P69" s="70"/>
-      <c r="Q69" s="70"/>
-      <c r="R69" s="70"/>
-      <c r="S69" s="70"/>
-      <c r="T69" s="70"/>
-      <c r="U69" s="70"/>
-      <c r="V69" s="70"/>
-      <c r="W69" s="70"/>
-      <c r="X69" s="70"/>
-      <c r="Y69" s="70"/>
-      <c r="Z69" s="70"/>
+      <c r="B69" s="83"/>
+      <c r="C69" s="83"/>
+      <c r="D69" s="83"/>
+      <c r="E69" s="83"/>
+      <c r="F69" s="83"/>
+      <c r="G69" s="83"/>
+      <c r="H69" s="83"/>
+      <c r="I69" s="83"/>
+      <c r="J69" s="83"/>
+      <c r="K69" s="83"/>
+      <c r="L69" s="83"/>
+      <c r="M69" s="83"/>
+      <c r="N69" s="83"/>
+      <c r="O69" s="83"/>
+      <c r="P69" s="83"/>
+      <c r="Q69" s="83"/>
+      <c r="R69" s="83"/>
+      <c r="S69" s="83"/>
+      <c r="T69" s="83"/>
+      <c r="U69" s="83"/>
+      <c r="V69" s="83"/>
+      <c r="W69" s="83"/>
+      <c r="X69" s="83"/>
+      <c r="Y69" s="83"/>
+      <c r="Z69" s="83"/>
     </row>
     <row r="70" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A70" s="72" t="s">
+      <c r="A70" s="84" t="s">
         <v>513</v>
       </c>
-      <c r="B70" s="72"/>
-      <c r="C70" s="72"/>
-      <c r="D70" s="72"/>
-      <c r="E70" s="72"/>
-      <c r="F70" s="72"/>
-      <c r="G70" s="72"/>
-      <c r="H70" s="72"/>
-      <c r="I70" s="72"/>
-      <c r="J70" s="72"/>
-      <c r="K70" s="72"/>
-      <c r="L70" s="72"/>
-      <c r="M70" s="72"/>
-      <c r="N70" s="72"/>
-      <c r="O70" s="72"/>
-      <c r="P70" s="72"/>
-      <c r="Q70" s="72"/>
-      <c r="R70" s="72"/>
-      <c r="S70" s="72"/>
-      <c r="T70" s="72"/>
-      <c r="U70" s="72"/>
-      <c r="V70" s="72"/>
-      <c r="W70" s="72"/>
-      <c r="X70" s="72"/>
-      <c r="Y70" s="72"/>
-      <c r="Z70" s="72"/>
+      <c r="B70" s="84"/>
+      <c r="C70" s="84"/>
+      <c r="D70" s="84"/>
+      <c r="E70" s="84"/>
+      <c r="F70" s="84"/>
+      <c r="G70" s="84"/>
+      <c r="H70" s="84"/>
+      <c r="I70" s="84"/>
+      <c r="J70" s="84"/>
+      <c r="K70" s="84"/>
+      <c r="L70" s="84"/>
+      <c r="M70" s="84"/>
+      <c r="N70" s="84"/>
+      <c r="O70" s="84"/>
+      <c r="P70" s="84"/>
+      <c r="Q70" s="84"/>
+      <c r="R70" s="84"/>
+      <c r="S70" s="84"/>
+      <c r="T70" s="84"/>
+      <c r="U70" s="84"/>
+      <c r="V70" s="84"/>
+      <c r="W70" s="84"/>
+      <c r="X70" s="84"/>
+      <c r="Y70" s="84"/>
+      <c r="Z70" s="84"/>
     </row>
     <row r="71" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A71" s="68" t="s">
+      <c r="A71" s="82" t="s">
         <v>514</v>
       </c>
-      <c r="B71" s="68"/>
-      <c r="C71" s="68"/>
-      <c r="D71" s="68"/>
-      <c r="E71" s="68"/>
-      <c r="F71" s="68"/>
-      <c r="G71" s="68"/>
-      <c r="H71" s="68"/>
-      <c r="I71" s="68"/>
-      <c r="J71" s="68"/>
-      <c r="K71" s="68"/>
-      <c r="L71" s="68"/>
-      <c r="M71" s="68"/>
-      <c r="N71" s="68"/>
-      <c r="O71" s="68"/>
-      <c r="P71" s="68"/>
-      <c r="Q71" s="68"/>
-      <c r="R71" s="68"/>
-      <c r="S71" s="68"/>
-      <c r="T71" s="68"/>
-      <c r="U71" s="68"/>
-      <c r="V71" s="68"/>
-      <c r="W71" s="68"/>
-      <c r="X71" s="68"/>
-      <c r="Y71" s="68"/>
-      <c r="Z71" s="68"/>
+      <c r="B71" s="82"/>
+      <c r="C71" s="82"/>
+      <c r="D71" s="82"/>
+      <c r="E71" s="82"/>
+      <c r="F71" s="82"/>
+      <c r="G71" s="82"/>
+      <c r="H71" s="82"/>
+      <c r="I71" s="82"/>
+      <c r="J71" s="82"/>
+      <c r="K71" s="82"/>
+      <c r="L71" s="82"/>
+      <c r="M71" s="82"/>
+      <c r="N71" s="82"/>
+      <c r="O71" s="82"/>
+      <c r="P71" s="82"/>
+      <c r="Q71" s="82"/>
+      <c r="R71" s="82"/>
+      <c r="S71" s="82"/>
+      <c r="T71" s="82"/>
+      <c r="U71" s="82"/>
+      <c r="V71" s="82"/>
+      <c r="W71" s="82"/>
+      <c r="X71" s="82"/>
+      <c r="Y71" s="82"/>
+      <c r="Z71" s="82"/>
     </row>
     <row r="72" spans="1:26" s="65" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A72" s="71" t="s">
+      <c r="A72" s="85" t="s">
         <v>515</v>
       </c>
-      <c r="B72" s="71"/>
-      <c r="C72" s="71"/>
-      <c r="D72" s="71"/>
-      <c r="E72" s="71"/>
-      <c r="F72" s="71"/>
-      <c r="G72" s="71"/>
-      <c r="H72" s="71"/>
-      <c r="I72" s="71"/>
-      <c r="J72" s="71"/>
-      <c r="K72" s="71"/>
-      <c r="L72" s="71"/>
-      <c r="M72" s="71"/>
-      <c r="N72" s="71"/>
-      <c r="O72" s="71"/>
-      <c r="P72" s="71"/>
-      <c r="Q72" s="71"/>
-      <c r="R72" s="71"/>
-      <c r="S72" s="71"/>
-      <c r="T72" s="71"/>
-      <c r="U72" s="71"/>
-      <c r="V72" s="71"/>
-      <c r="W72" s="71"/>
-      <c r="X72" s="71"/>
-      <c r="Y72" s="71"/>
-      <c r="Z72" s="71"/>
+      <c r="B72" s="85"/>
+      <c r="C72" s="85"/>
+      <c r="D72" s="85"/>
+      <c r="E72" s="85"/>
+      <c r="F72" s="85"/>
+      <c r="G72" s="85"/>
+      <c r="H72" s="85"/>
+      <c r="I72" s="85"/>
+      <c r="J72" s="85"/>
+      <c r="K72" s="85"/>
+      <c r="L72" s="85"/>
+      <c r="M72" s="85"/>
+      <c r="N72" s="85"/>
+      <c r="O72" s="85"/>
+      <c r="P72" s="85"/>
+      <c r="Q72" s="85"/>
+      <c r="R72" s="85"/>
+      <c r="S72" s="85"/>
+      <c r="T72" s="85"/>
+      <c r="U72" s="85"/>
+      <c r="V72" s="85"/>
+      <c r="W72" s="85"/>
+      <c r="X72" s="85"/>
+      <c r="Y72" s="85"/>
+      <c r="Z72" s="85"/>
     </row>
     <row r="73" spans="1:26" s="65" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A73" s="70" t="s">
+      <c r="A73" s="83" t="s">
         <v>516</v>
       </c>
-      <c r="B73" s="70"/>
-      <c r="C73" s="70"/>
-      <c r="D73" s="70"/>
-      <c r="E73" s="70"/>
-      <c r="F73" s="70"/>
-      <c r="G73" s="70"/>
-      <c r="H73" s="70"/>
-      <c r="I73" s="70"/>
-      <c r="J73" s="70"/>
-      <c r="K73" s="70"/>
-      <c r="L73" s="70"/>
-      <c r="M73" s="70"/>
-      <c r="N73" s="70"/>
-      <c r="O73" s="70"/>
-      <c r="P73" s="70"/>
-      <c r="Q73" s="70"/>
-      <c r="R73" s="70"/>
-      <c r="S73" s="70"/>
-      <c r="T73" s="70"/>
-      <c r="U73" s="70"/>
-      <c r="V73" s="70"/>
-      <c r="W73" s="70"/>
-      <c r="X73" s="70"/>
-      <c r="Y73" s="70"/>
-      <c r="Z73" s="70"/>
+      <c r="B73" s="83"/>
+      <c r="C73" s="83"/>
+      <c r="D73" s="83"/>
+      <c r="E73" s="83"/>
+      <c r="F73" s="83"/>
+      <c r="G73" s="83"/>
+      <c r="H73" s="83"/>
+      <c r="I73" s="83"/>
+      <c r="J73" s="83"/>
+      <c r="K73" s="83"/>
+      <c r="L73" s="83"/>
+      <c r="M73" s="83"/>
+      <c r="N73" s="83"/>
+      <c r="O73" s="83"/>
+      <c r="P73" s="83"/>
+      <c r="Q73" s="83"/>
+      <c r="R73" s="83"/>
+      <c r="S73" s="83"/>
+      <c r="T73" s="83"/>
+      <c r="U73" s="83"/>
+      <c r="V73" s="83"/>
+      <c r="W73" s="83"/>
+      <c r="X73" s="83"/>
+      <c r="Y73" s="83"/>
+      <c r="Z73" s="83"/>
     </row>
     <row r="74" spans="1:26" s="65" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A74" s="68" t="s">
+      <c r="A74" s="82" t="s">
         <v>517</v>
       </c>
-      <c r="B74" s="68"/>
-      <c r="C74" s="68"/>
-      <c r="D74" s="68"/>
-      <c r="E74" s="68"/>
-      <c r="F74" s="68"/>
-      <c r="G74" s="68"/>
-      <c r="H74" s="68"/>
-      <c r="I74" s="68"/>
-      <c r="J74" s="68"/>
-      <c r="K74" s="68"/>
-      <c r="L74" s="68"/>
-      <c r="M74" s="68"/>
-      <c r="N74" s="68"/>
-      <c r="O74" s="68"/>
-      <c r="P74" s="68"/>
-      <c r="Q74" s="68"/>
-      <c r="R74" s="68"/>
-      <c r="S74" s="68"/>
-      <c r="T74" s="68"/>
-      <c r="U74" s="68"/>
-      <c r="V74" s="68"/>
-      <c r="W74" s="68"/>
-      <c r="X74" s="68"/>
-      <c r="Y74" s="68"/>
-      <c r="Z74" s="68"/>
+      <c r="B74" s="82"/>
+      <c r="C74" s="82"/>
+      <c r="D74" s="82"/>
+      <c r="E74" s="82"/>
+      <c r="F74" s="82"/>
+      <c r="G74" s="82"/>
+      <c r="H74" s="82"/>
+      <c r="I74" s="82"/>
+      <c r="J74" s="82"/>
+      <c r="K74" s="82"/>
+      <c r="L74" s="82"/>
+      <c r="M74" s="82"/>
+      <c r="N74" s="82"/>
+      <c r="O74" s="82"/>
+      <c r="P74" s="82"/>
+      <c r="Q74" s="82"/>
+      <c r="R74" s="82"/>
+      <c r="S74" s="82"/>
+      <c r="T74" s="82"/>
+      <c r="U74" s="82"/>
+      <c r="V74" s="82"/>
+      <c r="W74" s="82"/>
+      <c r="X74" s="82"/>
+      <c r="Y74" s="82"/>
+      <c r="Z74" s="82"/>
     </row>
     <row r="75" spans="1:26" s="65" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A75" s="68" t="s">
+      <c r="A75" s="82" t="s">
         <v>518</v>
       </c>
-      <c r="B75" s="68"/>
-      <c r="C75" s="68"/>
-      <c r="D75" s="68"/>
-      <c r="E75" s="68"/>
-      <c r="F75" s="68"/>
-      <c r="G75" s="68"/>
-      <c r="H75" s="68"/>
-      <c r="I75" s="68"/>
-      <c r="J75" s="68"/>
-      <c r="K75" s="68"/>
-      <c r="L75" s="68"/>
-      <c r="M75" s="68"/>
-      <c r="N75" s="68"/>
-      <c r="O75" s="68"/>
-      <c r="P75" s="68"/>
-      <c r="Q75" s="68"/>
-      <c r="R75" s="68"/>
-      <c r="S75" s="68"/>
-      <c r="T75" s="68"/>
-      <c r="U75" s="68"/>
-      <c r="V75" s="68"/>
-      <c r="W75" s="68"/>
-      <c r="X75" s="68"/>
-      <c r="Y75" s="68"/>
-      <c r="Z75" s="68"/>
+      <c r="B75" s="82"/>
+      <c r="C75" s="82"/>
+      <c r="D75" s="82"/>
+      <c r="E75" s="82"/>
+      <c r="F75" s="82"/>
+      <c r="G75" s="82"/>
+      <c r="H75" s="82"/>
+      <c r="I75" s="82"/>
+      <c r="J75" s="82"/>
+      <c r="K75" s="82"/>
+      <c r="L75" s="82"/>
+      <c r="M75" s="82"/>
+      <c r="N75" s="82"/>
+      <c r="O75" s="82"/>
+      <c r="P75" s="82"/>
+      <c r="Q75" s="82"/>
+      <c r="R75" s="82"/>
+      <c r="S75" s="82"/>
+      <c r="T75" s="82"/>
+      <c r="U75" s="82"/>
+      <c r="V75" s="82"/>
+      <c r="W75" s="82"/>
+      <c r="X75" s="82"/>
+      <c r="Y75" s="82"/>
+      <c r="Z75" s="82"/>
     </row>
     <row r="76" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A76" s="68" t="s">
+      <c r="A76" s="82" t="s">
         <v>519</v>
       </c>
-      <c r="B76" s="68"/>
-      <c r="C76" s="68"/>
-      <c r="D76" s="68"/>
-      <c r="E76" s="68"/>
-      <c r="F76" s="68"/>
-      <c r="G76" s="68"/>
-      <c r="H76" s="68"/>
-      <c r="I76" s="68"/>
-      <c r="J76" s="68"/>
-      <c r="K76" s="68"/>
-      <c r="L76" s="68"/>
-      <c r="M76" s="68"/>
-      <c r="N76" s="68"/>
-      <c r="O76" s="68"/>
-      <c r="P76" s="68"/>
-      <c r="Q76" s="68"/>
-      <c r="R76" s="68"/>
-      <c r="S76" s="68"/>
-      <c r="T76" s="68"/>
-      <c r="U76" s="68"/>
-      <c r="V76" s="68"/>
-      <c r="W76" s="68"/>
-      <c r="X76" s="68"/>
-      <c r="Y76" s="68"/>
-      <c r="Z76" s="68"/>
+      <c r="B76" s="82"/>
+      <c r="C76" s="82"/>
+      <c r="D76" s="82"/>
+      <c r="E76" s="82"/>
+      <c r="F76" s="82"/>
+      <c r="G76" s="82"/>
+      <c r="H76" s="82"/>
+      <c r="I76" s="82"/>
+      <c r="J76" s="82"/>
+      <c r="K76" s="82"/>
+      <c r="L76" s="82"/>
+      <c r="M76" s="82"/>
+      <c r="N76" s="82"/>
+      <c r="O76" s="82"/>
+      <c r="P76" s="82"/>
+      <c r="Q76" s="82"/>
+      <c r="R76" s="82"/>
+      <c r="S76" s="82"/>
+      <c r="T76" s="82"/>
+      <c r="U76" s="82"/>
+      <c r="V76" s="82"/>
+      <c r="W76" s="82"/>
+      <c r="X76" s="82"/>
+      <c r="Y76" s="82"/>
+      <c r="Z76" s="82"/>
     </row>
     <row r="77" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A77" s="70" t="s">
+      <c r="A77" s="83" t="s">
         <v>520</v>
       </c>
-      <c r="B77" s="70"/>
-      <c r="C77" s="70"/>
-      <c r="D77" s="70"/>
-      <c r="E77" s="70"/>
-      <c r="F77" s="70"/>
-      <c r="G77" s="70"/>
-      <c r="H77" s="70"/>
-      <c r="I77" s="70"/>
-      <c r="J77" s="70"/>
-      <c r="K77" s="70"/>
-      <c r="L77" s="70"/>
-      <c r="M77" s="70"/>
-      <c r="N77" s="70"/>
-      <c r="O77" s="70"/>
-      <c r="P77" s="70"/>
-      <c r="Q77" s="70"/>
-      <c r="R77" s="70"/>
-      <c r="S77" s="70"/>
-      <c r="T77" s="70"/>
-      <c r="U77" s="70"/>
-      <c r="V77" s="70"/>
-      <c r="W77" s="70"/>
-      <c r="X77" s="70"/>
-      <c r="Y77" s="70"/>
-      <c r="Z77" s="70"/>
+      <c r="B77" s="83"/>
+      <c r="C77" s="83"/>
+      <c r="D77" s="83"/>
+      <c r="E77" s="83"/>
+      <c r="F77" s="83"/>
+      <c r="G77" s="83"/>
+      <c r="H77" s="83"/>
+      <c r="I77" s="83"/>
+      <c r="J77" s="83"/>
+      <c r="K77" s="83"/>
+      <c r="L77" s="83"/>
+      <c r="M77" s="83"/>
+      <c r="N77" s="83"/>
+      <c r="O77" s="83"/>
+      <c r="P77" s="83"/>
+      <c r="Q77" s="83"/>
+      <c r="R77" s="83"/>
+      <c r="S77" s="83"/>
+      <c r="T77" s="83"/>
+      <c r="U77" s="83"/>
+      <c r="V77" s="83"/>
+      <c r="W77" s="83"/>
+      <c r="X77" s="83"/>
+      <c r="Y77" s="83"/>
+      <c r="Z77" s="83"/>
     </row>
     <row r="78" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A78" s="68" t="s">
+      <c r="A78" s="82" t="s">
         <v>521</v>
       </c>
-      <c r="B78" s="68"/>
-      <c r="C78" s="68"/>
-      <c r="D78" s="68"/>
-      <c r="E78" s="68"/>
-      <c r="F78" s="68"/>
-      <c r="G78" s="68"/>
-      <c r="H78" s="68"/>
-      <c r="I78" s="68"/>
-      <c r="J78" s="68"/>
-      <c r="K78" s="68"/>
-      <c r="L78" s="68"/>
-      <c r="M78" s="68"/>
-      <c r="N78" s="68"/>
-      <c r="O78" s="68"/>
-      <c r="P78" s="68"/>
-      <c r="Q78" s="68"/>
-      <c r="R78" s="68"/>
-      <c r="S78" s="68"/>
-      <c r="T78" s="68"/>
-      <c r="U78" s="68"/>
-      <c r="V78" s="68"/>
-      <c r="W78" s="68"/>
-      <c r="X78" s="68"/>
-      <c r="Y78" s="68"/>
-      <c r="Z78" s="68"/>
+      <c r="B78" s="82"/>
+      <c r="C78" s="82"/>
+      <c r="D78" s="82"/>
+      <c r="E78" s="82"/>
+      <c r="F78" s="82"/>
+      <c r="G78" s="82"/>
+      <c r="H78" s="82"/>
+      <c r="I78" s="82"/>
+      <c r="J78" s="82"/>
+      <c r="K78" s="82"/>
+      <c r="L78" s="82"/>
+      <c r="M78" s="82"/>
+      <c r="N78" s="82"/>
+      <c r="O78" s="82"/>
+      <c r="P78" s="82"/>
+      <c r="Q78" s="82"/>
+      <c r="R78" s="82"/>
+      <c r="S78" s="82"/>
+      <c r="T78" s="82"/>
+      <c r="U78" s="82"/>
+      <c r="V78" s="82"/>
+      <c r="W78" s="82"/>
+      <c r="X78" s="82"/>
+      <c r="Y78" s="82"/>
+      <c r="Z78" s="82"/>
     </row>
     <row r="79" spans="1:26" s="65" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A79" s="68" t="s">
+      <c r="A79" s="82" t="s">
         <v>519</v>
       </c>
-      <c r="B79" s="68"/>
-      <c r="C79" s="68"/>
-      <c r="D79" s="68"/>
-      <c r="E79" s="68"/>
-      <c r="F79" s="68"/>
-      <c r="G79" s="68"/>
-      <c r="H79" s="68"/>
-      <c r="I79" s="68"/>
-      <c r="J79" s="68"/>
-      <c r="K79" s="68"/>
-      <c r="L79" s="68"/>
-      <c r="M79" s="68"/>
-      <c r="N79" s="68"/>
-      <c r="O79" s="68"/>
-      <c r="P79" s="68"/>
-      <c r="Q79" s="68"/>
-      <c r="R79" s="68"/>
-      <c r="S79" s="68"/>
-      <c r="T79" s="68"/>
-      <c r="U79" s="68"/>
-      <c r="V79" s="68"/>
-      <c r="W79" s="68"/>
-      <c r="X79" s="68"/>
-      <c r="Y79" s="68"/>
-      <c r="Z79" s="68"/>
+      <c r="B79" s="82"/>
+      <c r="C79" s="82"/>
+      <c r="D79" s="82"/>
+      <c r="E79" s="82"/>
+      <c r="F79" s="82"/>
+      <c r="G79" s="82"/>
+      <c r="H79" s="82"/>
+      <c r="I79" s="82"/>
+      <c r="J79" s="82"/>
+      <c r="K79" s="82"/>
+      <c r="L79" s="82"/>
+      <c r="M79" s="82"/>
+      <c r="N79" s="82"/>
+      <c r="O79" s="82"/>
+      <c r="P79" s="82"/>
+      <c r="Q79" s="82"/>
+      <c r="R79" s="82"/>
+      <c r="S79" s="82"/>
+      <c r="T79" s="82"/>
+      <c r="U79" s="82"/>
+      <c r="V79" s="82"/>
+      <c r="W79" s="82"/>
+      <c r="X79" s="82"/>
+      <c r="Y79" s="82"/>
+      <c r="Z79" s="82"/>
     </row>
     <row r="80" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A80" s="71" t="s">
+      <c r="A80" s="85" t="s">
         <v>522</v>
       </c>
-      <c r="B80" s="71"/>
-      <c r="C80" s="71"/>
-      <c r="D80" s="71"/>
-      <c r="E80" s="71"/>
-      <c r="F80" s="71"/>
-      <c r="G80" s="71"/>
-      <c r="H80" s="71"/>
-      <c r="I80" s="71"/>
-      <c r="J80" s="71"/>
-      <c r="K80" s="71"/>
-      <c r="L80" s="71"/>
-      <c r="M80" s="71"/>
-      <c r="N80" s="71"/>
-      <c r="O80" s="71"/>
-      <c r="P80" s="71"/>
-      <c r="Q80" s="71"/>
-      <c r="R80" s="71"/>
-      <c r="S80" s="71"/>
-      <c r="T80" s="71"/>
-      <c r="U80" s="71"/>
-      <c r="V80" s="71"/>
-      <c r="W80" s="71"/>
-      <c r="X80" s="71"/>
-      <c r="Y80" s="71"/>
-      <c r="Z80" s="71"/>
+      <c r="B80" s="85"/>
+      <c r="C80" s="85"/>
+      <c r="D80" s="85"/>
+      <c r="E80" s="85"/>
+      <c r="F80" s="85"/>
+      <c r="G80" s="85"/>
+      <c r="H80" s="85"/>
+      <c r="I80" s="85"/>
+      <c r="J80" s="85"/>
+      <c r="K80" s="85"/>
+      <c r="L80" s="85"/>
+      <c r="M80" s="85"/>
+      <c r="N80" s="85"/>
+      <c r="O80" s="85"/>
+      <c r="P80" s="85"/>
+      <c r="Q80" s="85"/>
+      <c r="R80" s="85"/>
+      <c r="S80" s="85"/>
+      <c r="T80" s="85"/>
+      <c r="U80" s="85"/>
+      <c r="V80" s="85"/>
+      <c r="W80" s="85"/>
+      <c r="X80" s="85"/>
+      <c r="Y80" s="85"/>
+      <c r="Z80" s="85"/>
     </row>
     <row r="81" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A81" s="68" t="s">
+      <c r="A81" s="82" t="s">
         <v>523</v>
       </c>
-      <c r="B81" s="68"/>
-      <c r="C81" s="68"/>
-      <c r="D81" s="68"/>
-      <c r="E81" s="68"/>
-      <c r="F81" s="68"/>
-      <c r="G81" s="68"/>
-      <c r="H81" s="68"/>
-      <c r="I81" s="68"/>
-      <c r="J81" s="68"/>
-      <c r="K81" s="68"/>
-      <c r="L81" s="68"/>
-      <c r="M81" s="68"/>
-      <c r="N81" s="68"/>
-      <c r="O81" s="68"/>
-      <c r="P81" s="68"/>
-      <c r="Q81" s="68"/>
-      <c r="R81" s="68"/>
-      <c r="S81" s="68"/>
-      <c r="T81" s="68"/>
-      <c r="U81" s="68"/>
-      <c r="V81" s="68"/>
-      <c r="W81" s="68"/>
-      <c r="X81" s="68"/>
-      <c r="Y81" s="68"/>
-      <c r="Z81" s="68"/>
+      <c r="B81" s="82"/>
+      <c r="C81" s="82"/>
+      <c r="D81" s="82"/>
+      <c r="E81" s="82"/>
+      <c r="F81" s="82"/>
+      <c r="G81" s="82"/>
+      <c r="H81" s="82"/>
+      <c r="I81" s="82"/>
+      <c r="J81" s="82"/>
+      <c r="K81" s="82"/>
+      <c r="L81" s="82"/>
+      <c r="M81" s="82"/>
+      <c r="N81" s="82"/>
+      <c r="O81" s="82"/>
+      <c r="P81" s="82"/>
+      <c r="Q81" s="82"/>
+      <c r="R81" s="82"/>
+      <c r="S81" s="82"/>
+      <c r="T81" s="82"/>
+      <c r="U81" s="82"/>
+      <c r="V81" s="82"/>
+      <c r="W81" s="82"/>
+      <c r="X81" s="82"/>
+      <c r="Y81" s="82"/>
+      <c r="Z81" s="82"/>
     </row>
     <row r="82" spans="1:26" s="64" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A82" s="68" t="s">
+      <c r="A82" s="82" t="s">
         <v>524</v>
       </c>
-      <c r="B82" s="68"/>
-      <c r="C82" s="68"/>
-      <c r="D82" s="68"/>
-      <c r="E82" s="68"/>
-      <c r="F82" s="68"/>
-      <c r="G82" s="68"/>
-      <c r="H82" s="68"/>
-      <c r="I82" s="68"/>
-      <c r="J82" s="68"/>
-      <c r="K82" s="68"/>
-      <c r="L82" s="68"/>
-      <c r="M82" s="68"/>
-      <c r="N82" s="68"/>
-      <c r="O82" s="68"/>
-      <c r="P82" s="68"/>
-      <c r="Q82" s="68"/>
-      <c r="R82" s="68"/>
-      <c r="S82" s="68"/>
-      <c r="T82" s="68"/>
-      <c r="U82" s="68"/>
-      <c r="V82" s="68"/>
-      <c r="W82" s="68"/>
-      <c r="X82" s="68"/>
-      <c r="Y82" s="68"/>
-      <c r="Z82" s="68"/>
+      <c r="B82" s="82"/>
+      <c r="C82" s="82"/>
+      <c r="D82" s="82"/>
+      <c r="E82" s="82"/>
+      <c r="F82" s="82"/>
+      <c r="G82" s="82"/>
+      <c r="H82" s="82"/>
+      <c r="I82" s="82"/>
+      <c r="J82" s="82"/>
+      <c r="K82" s="82"/>
+      <c r="L82" s="82"/>
+      <c r="M82" s="82"/>
+      <c r="N82" s="82"/>
+      <c r="O82" s="82"/>
+      <c r="P82" s="82"/>
+      <c r="Q82" s="82"/>
+      <c r="R82" s="82"/>
+      <c r="S82" s="82"/>
+      <c r="T82" s="82"/>
+      <c r="U82" s="82"/>
+      <c r="V82" s="82"/>
+      <c r="W82" s="82"/>
+      <c r="X82" s="82"/>
+      <c r="Y82" s="82"/>
+      <c r="Z82" s="82"/>
     </row>
     <row r="83" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A83" s="68" t="s">
+      <c r="A83" s="82" t="s">
         <v>525</v>
       </c>
-      <c r="B83" s="68"/>
-      <c r="C83" s="68"/>
-      <c r="D83" s="68"/>
-      <c r="E83" s="68"/>
-      <c r="F83" s="68"/>
-      <c r="G83" s="68"/>
-      <c r="H83" s="68"/>
-      <c r="I83" s="68"/>
-      <c r="J83" s="68"/>
-      <c r="K83" s="68"/>
-      <c r="L83" s="68"/>
-      <c r="M83" s="68"/>
-      <c r="N83" s="68"/>
-      <c r="O83" s="68"/>
-      <c r="P83" s="68"/>
-      <c r="Q83" s="68"/>
-      <c r="R83" s="68"/>
-      <c r="S83" s="68"/>
-      <c r="T83" s="68"/>
-      <c r="U83" s="68"/>
-      <c r="V83" s="68"/>
-      <c r="W83" s="68"/>
-      <c r="X83" s="68"/>
-      <c r="Y83" s="68"/>
-      <c r="Z83" s="68"/>
+      <c r="B83" s="82"/>
+      <c r="C83" s="82"/>
+      <c r="D83" s="82"/>
+      <c r="E83" s="82"/>
+      <c r="F83" s="82"/>
+      <c r="G83" s="82"/>
+      <c r="H83" s="82"/>
+      <c r="I83" s="82"/>
+      <c r="J83" s="82"/>
+      <c r="K83" s="82"/>
+      <c r="L83" s="82"/>
+      <c r="M83" s="82"/>
+      <c r="N83" s="82"/>
+      <c r="O83" s="82"/>
+      <c r="P83" s="82"/>
+      <c r="Q83" s="82"/>
+      <c r="R83" s="82"/>
+      <c r="S83" s="82"/>
+      <c r="T83" s="82"/>
+      <c r="U83" s="82"/>
+      <c r="V83" s="82"/>
+      <c r="W83" s="82"/>
+      <c r="X83" s="82"/>
+      <c r="Y83" s="82"/>
+      <c r="Z83" s="82"/>
     </row>
     <row r="84" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A84" s="69" t="s">
+      <c r="A84" s="86" t="s">
         <v>526</v>
       </c>
-      <c r="B84" s="69"/>
-      <c r="C84" s="69"/>
-      <c r="D84" s="69"/>
-      <c r="E84" s="69"/>
-      <c r="F84" s="69"/>
-      <c r="G84" s="69"/>
-      <c r="H84" s="69"/>
-      <c r="I84" s="69"/>
-      <c r="J84" s="69"/>
-      <c r="K84" s="69"/>
-      <c r="L84" s="69"/>
-      <c r="M84" s="69"/>
-      <c r="N84" s="69"/>
-      <c r="O84" s="69"/>
-      <c r="P84" s="69"/>
-      <c r="Q84" s="69"/>
-      <c r="R84" s="69"/>
-      <c r="S84" s="69"/>
-      <c r="T84" s="69"/>
-      <c r="U84" s="69"/>
-      <c r="V84" s="69"/>
-      <c r="W84" s="69"/>
-      <c r="X84" s="69"/>
-      <c r="Y84" s="69"/>
-      <c r="Z84" s="69"/>
+      <c r="B84" s="86"/>
+      <c r="C84" s="86"/>
+      <c r="D84" s="86"/>
+      <c r="E84" s="86"/>
+      <c r="F84" s="86"/>
+      <c r="G84" s="86"/>
+      <c r="H84" s="86"/>
+      <c r="I84" s="86"/>
+      <c r="J84" s="86"/>
+      <c r="K84" s="86"/>
+      <c r="L84" s="86"/>
+      <c r="M84" s="86"/>
+      <c r="N84" s="86"/>
+      <c r="O84" s="86"/>
+      <c r="P84" s="86"/>
+      <c r="Q84" s="86"/>
+      <c r="R84" s="86"/>
+      <c r="S84" s="86"/>
+      <c r="T84" s="86"/>
+      <c r="U84" s="86"/>
+      <c r="V84" s="86"/>
+      <c r="W84" s="86"/>
+      <c r="X84" s="86"/>
+      <c r="Y84" s="86"/>
+      <c r="Z84" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="A81:Z81"/>
+    <mergeCell ref="A82:Z82"/>
+    <mergeCell ref="A83:Z83"/>
+    <mergeCell ref="A84:Z84"/>
+    <mergeCell ref="A75:Z75"/>
+    <mergeCell ref="A76:Z76"/>
+    <mergeCell ref="A77:Z77"/>
+    <mergeCell ref="A78:Z78"/>
+    <mergeCell ref="A79:Z79"/>
+    <mergeCell ref="A80:Z80"/>
+    <mergeCell ref="A74:Z74"/>
+    <mergeCell ref="A63:Z63"/>
+    <mergeCell ref="A64:Z64"/>
+    <mergeCell ref="A65:Z65"/>
+    <mergeCell ref="A66:Z66"/>
+    <mergeCell ref="A67:Z67"/>
+    <mergeCell ref="A68:Z68"/>
+    <mergeCell ref="A69:Z69"/>
+    <mergeCell ref="A70:Z70"/>
+    <mergeCell ref="A71:Z71"/>
+    <mergeCell ref="A72:Z72"/>
+    <mergeCell ref="A73:Z73"/>
+    <mergeCell ref="A62:Z62"/>
+    <mergeCell ref="A51:Z51"/>
+    <mergeCell ref="A52:Z52"/>
+    <mergeCell ref="A53:Z53"/>
+    <mergeCell ref="A54:Z54"/>
+    <mergeCell ref="A55:Z55"/>
+    <mergeCell ref="A56:Z56"/>
+    <mergeCell ref="A57:Z57"/>
+    <mergeCell ref="A58:Z58"/>
+    <mergeCell ref="A59:Z59"/>
+    <mergeCell ref="A60:Z60"/>
+    <mergeCell ref="A61:Z61"/>
+    <mergeCell ref="A50:Z50"/>
+    <mergeCell ref="A39:Z39"/>
+    <mergeCell ref="A40:Z40"/>
+    <mergeCell ref="A41:Z41"/>
+    <mergeCell ref="A42:Z42"/>
+    <mergeCell ref="A43:Z43"/>
+    <mergeCell ref="A44:Z44"/>
+    <mergeCell ref="A45:Z45"/>
+    <mergeCell ref="A46:Z46"/>
+    <mergeCell ref="A47:Z47"/>
+    <mergeCell ref="A48:Z48"/>
+    <mergeCell ref="A49:Z49"/>
     <mergeCell ref="A38:Z38"/>
     <mergeCell ref="A1:AG1"/>
     <mergeCell ref="A28:Z28"/>
@@ -39492,52 +39538,6 @@
     <mergeCell ref="A35:Z35"/>
     <mergeCell ref="A36:Z36"/>
     <mergeCell ref="A37:Z37"/>
-    <mergeCell ref="A50:Z50"/>
-    <mergeCell ref="A39:Z39"/>
-    <mergeCell ref="A40:Z40"/>
-    <mergeCell ref="A41:Z41"/>
-    <mergeCell ref="A42:Z42"/>
-    <mergeCell ref="A43:Z43"/>
-    <mergeCell ref="A44:Z44"/>
-    <mergeCell ref="A45:Z45"/>
-    <mergeCell ref="A46:Z46"/>
-    <mergeCell ref="A47:Z47"/>
-    <mergeCell ref="A48:Z48"/>
-    <mergeCell ref="A49:Z49"/>
-    <mergeCell ref="A62:Z62"/>
-    <mergeCell ref="A51:Z51"/>
-    <mergeCell ref="A52:Z52"/>
-    <mergeCell ref="A53:Z53"/>
-    <mergeCell ref="A54:Z54"/>
-    <mergeCell ref="A55:Z55"/>
-    <mergeCell ref="A56:Z56"/>
-    <mergeCell ref="A57:Z57"/>
-    <mergeCell ref="A58:Z58"/>
-    <mergeCell ref="A59:Z59"/>
-    <mergeCell ref="A60:Z60"/>
-    <mergeCell ref="A61:Z61"/>
-    <mergeCell ref="A74:Z74"/>
-    <mergeCell ref="A63:Z63"/>
-    <mergeCell ref="A64:Z64"/>
-    <mergeCell ref="A65:Z65"/>
-    <mergeCell ref="A66:Z66"/>
-    <mergeCell ref="A67:Z67"/>
-    <mergeCell ref="A68:Z68"/>
-    <mergeCell ref="A69:Z69"/>
-    <mergeCell ref="A70:Z70"/>
-    <mergeCell ref="A71:Z71"/>
-    <mergeCell ref="A72:Z72"/>
-    <mergeCell ref="A73:Z73"/>
-    <mergeCell ref="A81:Z81"/>
-    <mergeCell ref="A82:Z82"/>
-    <mergeCell ref="A83:Z83"/>
-    <mergeCell ref="A84:Z84"/>
-    <mergeCell ref="A75:Z75"/>
-    <mergeCell ref="A76:Z76"/>
-    <mergeCell ref="A77:Z77"/>
-    <mergeCell ref="A78:Z78"/>
-    <mergeCell ref="A79:Z79"/>
-    <mergeCell ref="A80:Z80"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
   <pageSetup scale="42" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Allocate vehicle classes 3-6 to freight LDVs and 7-8 to freight HDVs
</commit_message>
<xml_diff>
--- a/InputData/trans/BAADTbVT/BAU Avg Annual Dist Traveled by Veh Type.xlsx
+++ b/InputData/trans/BAADTbVT/BAU Avg Annual Dist Traveled by Veh Type.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\United States\US-EPS\InputData\trans\BAADTbVT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-us\InputData\trans\BAADTbVT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12ECC897-6652-4FEC-9CB5-5FF7D2D3A8E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1635" yWindow="1245" windowWidth="20265" windowHeight="15810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1635" yWindow="1245" windowWidth="20265" windowHeight="15810"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -46,7 +45,7 @@
     <definedName name="ti_tbl_69" localSheetId="10">#REF!</definedName>
     <definedName name="ti_tbl_69">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -5021,7 +5020,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="9">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -6205,9 +6204,9 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="54">
       <alignment wrapText="1"/>
     </xf>
@@ -6271,160 +6270,160 @@
     </xf>
   </cellXfs>
   <cellStyles count="154">
-    <cellStyle name="20% - Accent1 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="20% - Accent2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="20% - Accent3 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="20% - Accent4 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="20% - Accent5 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="20% - Accent6 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="40% - Accent1 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="40% - Accent2 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="40% - Accent3 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="40% - Accent4 2" xfId="13" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="40% - Accent5 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="40% - Accent6 2" xfId="15" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="60% - Accent1 2" xfId="16" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="60% - Accent2 2" xfId="17" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="60% - Accent3 2" xfId="18" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="60% - Accent4 2" xfId="19" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="60% - Accent5 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="60% - Accent6 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Accent1 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="Accent2 2" xfId="23" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="Accent3 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="Accent4 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="Accent5 2" xfId="26" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="Accent6 2" xfId="27" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="Bad 2" xfId="28" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="Body: normal cell" xfId="29" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="Body: normal cell 2" xfId="30" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="Calculation 2" xfId="31" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="Check Cell 2" xfId="32" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="Column heading" xfId="33" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="Comma 2" xfId="34" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="Comma 2 2" xfId="35" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="Comma 3" xfId="36" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="Comma 4" xfId="37" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="Comma 5" xfId="38" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="Comma 6" xfId="39" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="Comma 7" xfId="40" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="Comma 8" xfId="41" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="Corner heading" xfId="42" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="Currency 2" xfId="43" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="Currency 3" xfId="44" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="Currency 3 2" xfId="45" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="Data" xfId="46" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="Data 2" xfId="47" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="Data no deci" xfId="48" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="Data Superscript" xfId="49" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
-    <cellStyle name="Data_1-1A-Regular" xfId="50" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
-    <cellStyle name="Explanatory Text 2" xfId="51" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="52" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="54" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="Footnotes: top row 2" xfId="55" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="Good 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
-    <cellStyle name="Header: bottom row" xfId="57" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="Header: bottom row 2" xfId="58" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
-    <cellStyle name="Heading 1 2" xfId="59" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="Heading 2 2" xfId="60" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="Heading 3 2" xfId="61" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
-    <cellStyle name="Heading 4 2" xfId="62" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
-    <cellStyle name="Hed Side" xfId="63" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="Hed Side 2" xfId="64" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
-    <cellStyle name="Hed Side bold" xfId="65" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
-    <cellStyle name="Hed Side Indent" xfId="66" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
-    <cellStyle name="Hed Side Regular" xfId="67" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
-    <cellStyle name="Hed Side_1-1A-Regular" xfId="68" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
-    <cellStyle name="Hed Top" xfId="69" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
-    <cellStyle name="Hed Top - SECTION" xfId="70" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
-    <cellStyle name="Hed Top_3-new4" xfId="71" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="20% - Accent1 2" xfId="4"/>
+    <cellStyle name="20% - Accent2 2" xfId="5"/>
+    <cellStyle name="20% - Accent3 2" xfId="6"/>
+    <cellStyle name="20% - Accent4 2" xfId="7"/>
+    <cellStyle name="20% - Accent5 2" xfId="8"/>
+    <cellStyle name="20% - Accent6 2" xfId="9"/>
+    <cellStyle name="40% - Accent1 2" xfId="10"/>
+    <cellStyle name="40% - Accent2 2" xfId="11"/>
+    <cellStyle name="40% - Accent3 2" xfId="12"/>
+    <cellStyle name="40% - Accent4 2" xfId="13"/>
+    <cellStyle name="40% - Accent5 2" xfId="14"/>
+    <cellStyle name="40% - Accent6 2" xfId="15"/>
+    <cellStyle name="60% - Accent1 2" xfId="16"/>
+    <cellStyle name="60% - Accent2 2" xfId="17"/>
+    <cellStyle name="60% - Accent3 2" xfId="18"/>
+    <cellStyle name="60% - Accent4 2" xfId="19"/>
+    <cellStyle name="60% - Accent5 2" xfId="20"/>
+    <cellStyle name="60% - Accent6 2" xfId="21"/>
+    <cellStyle name="Accent1 2" xfId="22"/>
+    <cellStyle name="Accent2 2" xfId="23"/>
+    <cellStyle name="Accent3 2" xfId="24"/>
+    <cellStyle name="Accent4 2" xfId="25"/>
+    <cellStyle name="Accent5 2" xfId="26"/>
+    <cellStyle name="Accent6 2" xfId="27"/>
+    <cellStyle name="Bad 2" xfId="28"/>
+    <cellStyle name="Body: normal cell" xfId="29"/>
+    <cellStyle name="Body: normal cell 2" xfId="30"/>
+    <cellStyle name="Calculation 2" xfId="31"/>
+    <cellStyle name="Check Cell 2" xfId="32"/>
+    <cellStyle name="Column heading" xfId="33"/>
+    <cellStyle name="Comma 2" xfId="34"/>
+    <cellStyle name="Comma 2 2" xfId="35"/>
+    <cellStyle name="Comma 3" xfId="36"/>
+    <cellStyle name="Comma 4" xfId="37"/>
+    <cellStyle name="Comma 5" xfId="38"/>
+    <cellStyle name="Comma 6" xfId="39"/>
+    <cellStyle name="Comma 7" xfId="40"/>
+    <cellStyle name="Comma 8" xfId="41"/>
+    <cellStyle name="Corner heading" xfId="42"/>
+    <cellStyle name="Currency 2" xfId="43"/>
+    <cellStyle name="Currency 3" xfId="44"/>
+    <cellStyle name="Currency 3 2" xfId="45"/>
+    <cellStyle name="Data" xfId="46"/>
+    <cellStyle name="Data 2" xfId="47"/>
+    <cellStyle name="Data no deci" xfId="48"/>
+    <cellStyle name="Data Superscript" xfId="49"/>
+    <cellStyle name="Data_1-1A-Regular" xfId="50"/>
+    <cellStyle name="Explanatory Text 2" xfId="51"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="52"/>
+    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="53"/>
+    <cellStyle name="Footnotes: top row" xfId="54"/>
+    <cellStyle name="Footnotes: top row 2" xfId="55"/>
+    <cellStyle name="Good 2" xfId="56"/>
+    <cellStyle name="Header: bottom row" xfId="57"/>
+    <cellStyle name="Header: bottom row 2" xfId="58"/>
+    <cellStyle name="Heading 1 2" xfId="59"/>
+    <cellStyle name="Heading 2 2" xfId="60"/>
+    <cellStyle name="Heading 3 2" xfId="61"/>
+    <cellStyle name="Heading 4 2" xfId="62"/>
+    <cellStyle name="Hed Side" xfId="63"/>
+    <cellStyle name="Hed Side 2" xfId="64"/>
+    <cellStyle name="Hed Side bold" xfId="65"/>
+    <cellStyle name="Hed Side Indent" xfId="66"/>
+    <cellStyle name="Hed Side Regular" xfId="67"/>
+    <cellStyle name="Hed Side_1-1A-Regular" xfId="68"/>
+    <cellStyle name="Hed Top" xfId="69"/>
+    <cellStyle name="Hed Top - SECTION" xfId="70"/>
+    <cellStyle name="Hed Top_3-new4" xfId="71"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="72" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
-    <cellStyle name="Input 2" xfId="73" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
-    <cellStyle name="Linked Cell 2" xfId="74" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
-    <cellStyle name="Neutral 2" xfId="75" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
+    <cellStyle name="Hyperlink 2" xfId="72"/>
+    <cellStyle name="Input 2" xfId="73"/>
+    <cellStyle name="Linked Cell 2" xfId="74"/>
+    <cellStyle name="Neutral 2" xfId="75"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="76" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
-    <cellStyle name="Normal 11" xfId="77" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
-    <cellStyle name="Normal 2 2" xfId="78" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
-    <cellStyle name="Normal 2 3" xfId="79" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="Normal 3 2" xfId="80" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
-    <cellStyle name="Normal 3 2 2" xfId="81" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
-    <cellStyle name="Normal 3 2 2 2" xfId="82" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
-    <cellStyle name="Normal 3 2 3" xfId="83" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
-    <cellStyle name="Normal 3 3" xfId="84" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
-    <cellStyle name="Normal 3 3 2" xfId="85" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
-    <cellStyle name="Normal 3 3 2 2" xfId="86" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
-    <cellStyle name="Normal 3 3 3" xfId="87" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="Normal 3 4" xfId="88" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
-    <cellStyle name="Normal 3 4 2" xfId="89" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
-    <cellStyle name="Normal 3 5" xfId="90" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
-    <cellStyle name="Normal 3 6" xfId="91" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
-    <cellStyle name="Normal 3 7" xfId="92" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
-    <cellStyle name="Normal 4" xfId="93" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
-    <cellStyle name="Normal 4 2" xfId="94" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
-    <cellStyle name="Normal 4 2 2" xfId="95" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
-    <cellStyle name="Normal 4 2 2 2" xfId="96" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
-    <cellStyle name="Normal 4 2 3" xfId="97" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
-    <cellStyle name="Normal 4 3" xfId="98" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
-    <cellStyle name="Normal 4 3 2" xfId="99" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
-    <cellStyle name="Normal 4 3 2 2" xfId="100" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
-    <cellStyle name="Normal 4 3 3" xfId="101" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
-    <cellStyle name="Normal 4 4" xfId="102" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
-    <cellStyle name="Normal 4 4 2" xfId="103" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
-    <cellStyle name="Normal 4 5" xfId="104" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
-    <cellStyle name="Normal 4 6" xfId="105" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
-    <cellStyle name="Normal 4 7" xfId="106" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
-    <cellStyle name="Normal 5" xfId="107" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
-    <cellStyle name="Normal 5 2" xfId="108" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
-    <cellStyle name="Normal 5 3" xfId="109" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
-    <cellStyle name="Normal 6" xfId="110" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
-    <cellStyle name="Normal 6 2" xfId="111" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
-    <cellStyle name="Normal 7" xfId="112" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
-    <cellStyle name="Normal 7 2" xfId="113" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
-    <cellStyle name="Normal 8" xfId="114" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
-    <cellStyle name="Normal 9" xfId="115" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
-    <cellStyle name="Note 2" xfId="116" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
-    <cellStyle name="Note 2 2" xfId="117" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
-    <cellStyle name="Output 2" xfId="118" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
-    <cellStyle name="Parent row" xfId="119" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
-    <cellStyle name="Parent row 2" xfId="120" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
-    <cellStyle name="Percent 2" xfId="121" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
-    <cellStyle name="Percent 2 2" xfId="122" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
-    <cellStyle name="Percent 3" xfId="123" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
-    <cellStyle name="Percent 3 2" xfId="124" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
-    <cellStyle name="Percent 4" xfId="125" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
-    <cellStyle name="Reference" xfId="126" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
-    <cellStyle name="Row heading" xfId="127" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
-    <cellStyle name="Source Hed" xfId="128" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
-    <cellStyle name="Source Letter" xfId="129" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
-    <cellStyle name="Source Superscript" xfId="130" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
-    <cellStyle name="Source Superscript 2" xfId="131" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
-    <cellStyle name="Source Text" xfId="132" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
-    <cellStyle name="Source Text 2" xfId="133" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
-    <cellStyle name="State" xfId="134" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
-    <cellStyle name="Superscript" xfId="135" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
-    <cellStyle name="Table Data" xfId="136" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
-    <cellStyle name="Table Head Top" xfId="137" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
-    <cellStyle name="Table Hed Side" xfId="138" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
-    <cellStyle name="Table title" xfId="139" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
-    <cellStyle name="Table title 2" xfId="140" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
-    <cellStyle name="Title 2" xfId="141" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
-    <cellStyle name="Title Text" xfId="142" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
-    <cellStyle name="Title Text 1" xfId="143" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
-    <cellStyle name="Title Text 2" xfId="144" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
-    <cellStyle name="Title-1" xfId="145" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
-    <cellStyle name="Title-2" xfId="146" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
-    <cellStyle name="Title-3" xfId="147" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
-    <cellStyle name="Total 2" xfId="148" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
-    <cellStyle name="Warning Text 2" xfId="149" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
-    <cellStyle name="Wrap" xfId="150" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
-    <cellStyle name="Wrap Bold" xfId="151" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
-    <cellStyle name="Wrap Title" xfId="152" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
-    <cellStyle name="Wrap_NTS99-~11" xfId="153" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
+    <cellStyle name="Normal 10" xfId="76"/>
+    <cellStyle name="Normal 11" xfId="77"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2 2" xfId="78"/>
+    <cellStyle name="Normal 2 3" xfId="79"/>
+    <cellStyle name="Normal 3" xfId="3"/>
+    <cellStyle name="Normal 3 2" xfId="80"/>
+    <cellStyle name="Normal 3 2 2" xfId="81"/>
+    <cellStyle name="Normal 3 2 2 2" xfId="82"/>
+    <cellStyle name="Normal 3 2 3" xfId="83"/>
+    <cellStyle name="Normal 3 3" xfId="84"/>
+    <cellStyle name="Normal 3 3 2" xfId="85"/>
+    <cellStyle name="Normal 3 3 2 2" xfId="86"/>
+    <cellStyle name="Normal 3 3 3" xfId="87"/>
+    <cellStyle name="Normal 3 4" xfId="88"/>
+    <cellStyle name="Normal 3 4 2" xfId="89"/>
+    <cellStyle name="Normal 3 5" xfId="90"/>
+    <cellStyle name="Normal 3 6" xfId="91"/>
+    <cellStyle name="Normal 3 7" xfId="92"/>
+    <cellStyle name="Normal 4" xfId="93"/>
+    <cellStyle name="Normal 4 2" xfId="94"/>
+    <cellStyle name="Normal 4 2 2" xfId="95"/>
+    <cellStyle name="Normal 4 2 2 2" xfId="96"/>
+    <cellStyle name="Normal 4 2 3" xfId="97"/>
+    <cellStyle name="Normal 4 3" xfId="98"/>
+    <cellStyle name="Normal 4 3 2" xfId="99"/>
+    <cellStyle name="Normal 4 3 2 2" xfId="100"/>
+    <cellStyle name="Normal 4 3 3" xfId="101"/>
+    <cellStyle name="Normal 4 4" xfId="102"/>
+    <cellStyle name="Normal 4 4 2" xfId="103"/>
+    <cellStyle name="Normal 4 5" xfId="104"/>
+    <cellStyle name="Normal 4 6" xfId="105"/>
+    <cellStyle name="Normal 4 7" xfId="106"/>
+    <cellStyle name="Normal 5" xfId="107"/>
+    <cellStyle name="Normal 5 2" xfId="108"/>
+    <cellStyle name="Normal 5 3" xfId="109"/>
+    <cellStyle name="Normal 6" xfId="110"/>
+    <cellStyle name="Normal 6 2" xfId="111"/>
+    <cellStyle name="Normal 7" xfId="112"/>
+    <cellStyle name="Normal 7 2" xfId="113"/>
+    <cellStyle name="Normal 8" xfId="114"/>
+    <cellStyle name="Normal 9" xfId="115"/>
+    <cellStyle name="Note 2" xfId="116"/>
+    <cellStyle name="Note 2 2" xfId="117"/>
+    <cellStyle name="Output 2" xfId="118"/>
+    <cellStyle name="Parent row" xfId="119"/>
+    <cellStyle name="Parent row 2" xfId="120"/>
+    <cellStyle name="Percent 2" xfId="121"/>
+    <cellStyle name="Percent 2 2" xfId="122"/>
+    <cellStyle name="Percent 3" xfId="123"/>
+    <cellStyle name="Percent 3 2" xfId="124"/>
+    <cellStyle name="Percent 4" xfId="125"/>
+    <cellStyle name="Reference" xfId="126"/>
+    <cellStyle name="Row heading" xfId="127"/>
+    <cellStyle name="Source Hed" xfId="128"/>
+    <cellStyle name="Source Letter" xfId="129"/>
+    <cellStyle name="Source Superscript" xfId="130"/>
+    <cellStyle name="Source Superscript 2" xfId="131"/>
+    <cellStyle name="Source Text" xfId="132"/>
+    <cellStyle name="Source Text 2" xfId="133"/>
+    <cellStyle name="State" xfId="134"/>
+    <cellStyle name="Superscript" xfId="135"/>
+    <cellStyle name="Table Data" xfId="136"/>
+    <cellStyle name="Table Head Top" xfId="137"/>
+    <cellStyle name="Table Hed Side" xfId="138"/>
+    <cellStyle name="Table title" xfId="139"/>
+    <cellStyle name="Table title 2" xfId="140"/>
+    <cellStyle name="Title 2" xfId="141"/>
+    <cellStyle name="Title Text" xfId="142"/>
+    <cellStyle name="Title Text 1" xfId="143"/>
+    <cellStyle name="Title Text 2" xfId="144"/>
+    <cellStyle name="Title-1" xfId="145"/>
+    <cellStyle name="Title-2" xfId="146"/>
+    <cellStyle name="Title-3" xfId="147"/>
+    <cellStyle name="Total 2" xfId="148"/>
+    <cellStyle name="Warning Text 2" xfId="149"/>
+    <cellStyle name="Wrap" xfId="150"/>
+    <cellStyle name="Wrap Bold" xfId="151"/>
+    <cellStyle name="Wrap Title" xfId="152"/>
+    <cellStyle name="Wrap_NTS99-~11" xfId="153"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -6677,23 +6676,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -6729,23 +6711,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -6921,16 +6886,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="51.5703125" customWidth="1"/>
+    <col min="2" max="2" width="51.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -7126,14 +7091,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" customWidth="1"/>
+    <col min="1" max="1" width="33.86328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -7176,7 +7141,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -7189,11 +7154,11 @@
       <selection pane="bottomRight" activeCell="AJ3" sqref="AJ3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="37.7109375" style="39" customWidth="1"/>
-    <col min="2" max="33" width="8.7109375" style="39" customWidth="1"/>
-    <col min="34" max="16384" width="9.140625" style="39"/>
+    <col min="1" max="1" width="37.73046875" style="39" customWidth="1"/>
+    <col min="2" max="33" width="8.73046875" style="39" customWidth="1"/>
+    <col min="34" max="16384" width="9.1328125" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" s="29" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
@@ -11806,22 +11771,22 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.86328125" customWidth="1"/>
+    <col min="2" max="2" width="16.73046875" customWidth="1"/>
+    <col min="3" max="3" width="12.59765625" customWidth="1"/>
+    <col min="4" max="4" width="14.1328125" customWidth="1"/>
+    <col min="5" max="5" width="16.73046875" customWidth="1"/>
+    <col min="6" max="6" width="16.265625" customWidth="1"/>
+    <col min="7" max="7" width="15.86328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -11832,7 +11797,7 @@
     <row r="2" spans="1:7">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="45">
+    <row r="3" spans="1:7" ht="42.75">
       <c r="A3" s="9" t="s">
         <v>20</v>
       </c>
@@ -12046,7 +12011,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -12056,14 +12021,14 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="14" customWidth="1"/>
+    <col min="1" max="1" width="16.59765625" style="14" customWidth="1"/>
     <col min="2" max="2" width="9" style="14" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="14"/>
+    <col min="3" max="16384" width="9.1328125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="30">
+    <row r="1" spans="1:34" ht="28.5">
       <c r="A1" s="9" t="s">
         <v>270</v>
       </c>
@@ -12999,23 +12964,23 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AG7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="14" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="14"/>
+    <col min="1" max="1" width="16.59765625" style="14" customWidth="1"/>
+    <col min="2" max="16384" width="9.1328125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="30">
+    <row r="1" spans="1:33" ht="28.5">
       <c r="A1" s="9" t="s">
         <v>270</v>
       </c>
@@ -13120,266 +13085,266 @@
       <c r="A2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="82">
-        <f>(INDEX('AEO 7'!19:19,MATCH(About!$B$39,'AEO 7'!$13:$13,0))+SUM(SUMIFS('AEO 49'!$10:$10,'AEO 49'!$5:$5,B1),SUMIFS('AEO 49'!$21:$21,'AEO 49'!$5:$5,B1),SUMIFS('AEO 49'!$32:$32,'AEO 49'!$5:$5,B1))-INDEX('AEO 46'!$B:$B,MATCH(B1,'AEO 46'!$A:$A,0)))*1000000000/SUM('SYVbT-freight'!$B$2:$H$2)</f>
-        <v>7697.457895331032</v>
+      <c r="B2" s="84">
+        <f>(INDEX('AEO 7'!19:19,MATCH(About!$B$39,'AEO 7'!$13:$13,0))+INDEX('AEO 49'!18:18,MATCH(B1,'AEO 49'!5:5,0))+INDEX('AEO 49'!29:29,MATCH(B1,'AEO 49'!5:5,0)))*1000000000/SUM('SYVbT-freight'!$B$2:$H$2)</f>
+        <v>9905.2133456774991</v>
       </c>
       <c r="C2" s="15">
         <f t="shared" ref="C2:C7" si="0">B2</f>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="D2" s="15">
         <f t="shared" ref="D2:AG7" si="1">C2</f>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="E2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="F2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="G2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="H2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="I2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="J2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="K2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="L2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="M2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="N2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="O2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="P2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="Q2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="R2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="S2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="T2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="U2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="V2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="W2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="X2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="Y2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="Z2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="AA2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="AB2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="AC2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="AD2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="AE2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="AF2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
       <c r="AG2" s="15">
         <f t="shared" si="1"/>
-        <v>7697.457895331032</v>
+        <v>9905.2133456774991</v>
       </c>
     </row>
     <row r="3" spans="1:33">
       <c r="A3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="82">
-        <f>(INDEX('AEO 7'!20:20,MATCH(About!$B$39,'AEO 7'!$13:$13,0))-SUM(SUMIFS('AEO 49'!$10:$10,'AEO 49'!$5:$5,B1),SUMIFS('AEO 49'!$21:$21,'AEO 49'!$5:$5,B1),SUMIFS('AEO 49'!$32:$32,'AEO 49'!$5:$5,B1))+INDEX('AEO 46'!$B$5:$B$38,MATCH('BAADTbVT-freight'!B1,'AEO 46'!$A$5:$A$38,0)))*1000000000/SUM('SYVbT-freight'!$B$3:$H$3)</f>
-        <v>20663.778690226536</v>
+      <c r="B3" s="84">
+        <f>(INDEX('AEO 49'!40:40,MATCH(About!$B$39,'AEO 49'!5:5,0)))*1000000000/SUM('SYVbT-freight'!$B$3:$H$3)</f>
+        <v>37032.719616765411</v>
       </c>
       <c r="C3" s="15">
         <f t="shared" si="0"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="D3" s="15">
         <f t="shared" ref="D3:Q3" si="2">C3</f>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="E3" s="15">
         <f t="shared" si="2"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="F3" s="15">
         <f t="shared" si="2"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="G3" s="15">
         <f t="shared" si="2"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="H3" s="15">
         <f t="shared" si="2"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="I3" s="15">
         <f t="shared" si="2"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="J3" s="15">
         <f t="shared" si="2"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="K3" s="15">
         <f t="shared" si="2"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="L3" s="15">
         <f t="shared" si="2"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="M3" s="15">
         <f t="shared" si="2"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="N3" s="15">
         <f t="shared" si="2"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="O3" s="15">
         <f t="shared" si="2"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="P3" s="15">
         <f t="shared" si="2"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="Q3" s="15">
         <f t="shared" si="2"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="R3" s="15">
         <f t="shared" si="1"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="S3" s="15">
         <f t="shared" si="1"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="T3" s="15">
         <f t="shared" si="1"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="U3" s="15">
         <f t="shared" si="1"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="V3" s="15">
         <f t="shared" si="1"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="W3" s="15">
         <f t="shared" si="1"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="X3" s="15">
         <f t="shared" si="1"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="Y3" s="15">
         <f t="shared" si="1"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="Z3" s="15">
         <f t="shared" si="1"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="AA3" s="15">
         <f t="shared" si="1"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="AB3" s="15">
         <f t="shared" si="1"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="AC3" s="15">
         <f t="shared" si="1"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="AD3" s="15">
         <f t="shared" si="1"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="AE3" s="15">
         <f t="shared" si="1"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="AF3" s="15">
         <f t="shared" si="1"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
       <c r="AG3" s="15">
         <f t="shared" si="1"/>
-        <v>20663.778690226536</v>
+        <v>37032.719616765411</v>
       </c>
     </row>
     <row r="4" spans="1:33">
@@ -13920,23 +13885,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H7"/>
+      <selection activeCell="B2" sqref="B2:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.86328125" customWidth="1"/>
+    <col min="2" max="2" width="24.59765625" customWidth="1"/>
+    <col min="3" max="3" width="20.86328125" customWidth="1"/>
+    <col min="4" max="4" width="18.265625" customWidth="1"/>
+    <col min="5" max="5" width="17.1328125" customWidth="1"/>
+    <col min="6" max="6" width="23.265625" customWidth="1"/>
+    <col min="7" max="7" width="19.265625" customWidth="1"/>
+    <col min="8" max="8" width="22.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -14133,23 +14098,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B2" sqref="B2:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.86328125" customWidth="1"/>
+    <col min="2" max="2" width="24.59765625" customWidth="1"/>
+    <col min="3" max="3" width="20.86328125" customWidth="1"/>
+    <col min="4" max="4" width="18.265625" customWidth="1"/>
+    <col min="5" max="5" width="17.1328125" customWidth="1"/>
+    <col min="6" max="6" width="23.265625" customWidth="1"/>
+    <col min="7" max="7" width="19.265625" customWidth="1"/>
+    <col min="8" max="8" width="20.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -14183,22 +14148,22 @@
         <v>5</v>
       </c>
       <c r="B2" s="25">
-        <v>0</v>
+        <v>84.000000000000014</v>
       </c>
       <c r="C2" s="25">
-        <v>11809.598</v>
+        <v>14866.598</v>
       </c>
       <c r="D2" s="25">
-        <v>12021582.539999999</v>
+        <v>11972117.539999999</v>
       </c>
       <c r="E2" s="25">
-        <v>0</v>
+        <v>9818361.2930000015</v>
       </c>
       <c r="F2" s="25">
         <v>0</v>
       </c>
       <c r="G2" s="25">
-        <v>1444.8510000000001</v>
+        <v>5402.8509999999997</v>
       </c>
       <c r="H2" s="58">
         <v>0</v>
@@ -14209,22 +14174,22 @@
         <v>6</v>
       </c>
       <c r="B3" s="58">
-        <v>84.000000000000014</v>
+        <v>0</v>
       </c>
       <c r="C3" s="58">
-        <v>46227</v>
+        <v>43170</v>
       </c>
       <c r="D3" s="58">
-        <v>0</v>
+        <v>49465</v>
       </c>
       <c r="E3" s="58">
-        <v>14786498.293000001</v>
+        <v>4968137</v>
       </c>
       <c r="F3" s="58">
         <v>202</v>
       </c>
       <c r="G3" s="25">
-        <v>7966.0000000000009</v>
+        <v>4008.0000000000005</v>
       </c>
       <c r="H3" s="25">
         <v>114</v>
@@ -14340,17 +14305,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.1328125" customWidth="1"/>
+    <col min="2" max="2" width="8.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37">
@@ -15148,16 +15113,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.86328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" s="1" customFormat="1">
@@ -15934,11 +15899,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B46" sqref="B46"/>
       <selection pane="topRight" activeCell="B46" sqref="B46"/>
       <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
@@ -15947,8 +15912,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.86328125" customWidth="1"/>
+    <col min="2" max="2" width="45.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15" customHeight="1" thickBot="1">
@@ -22370,14 +22335,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="17.265625" defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -22679,7 +22644,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM200"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -22690,13 +22655,13 @@
       <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="58"/>
-    <col min="2" max="2" width="116.5703125" style="76" customWidth="1"/>
-    <col min="3" max="3" width="53.140625" style="58" customWidth="1"/>
-    <col min="4" max="4" width="45.7109375" style="58" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="58"/>
+    <col min="1" max="1" width="9.1328125" style="58"/>
+    <col min="2" max="2" width="116.59765625" style="76" customWidth="1"/>
+    <col min="3" max="3" width="53.1328125" style="58" customWidth="1"/>
+    <col min="4" max="4" width="45.73046875" style="58" customWidth="1"/>
+    <col min="5" max="16384" width="9.1328125" style="58"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="15" customHeight="1" thickBot="1">
@@ -22825,31 +22790,31 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:38">
+    <row r="5" spans="1:38" ht="14.25">
       <c r="A5" s="58" t="s">
         <v>303</v>
       </c>
       <c r="B5" s="58"/>
     </row>
-    <row r="6" spans="1:38">
+    <row r="6" spans="1:38" ht="14.25">
       <c r="A6" s="58" t="s">
         <v>304</v>
       </c>
       <c r="B6" s="58"/>
     </row>
-    <row r="7" spans="1:38">
+    <row r="7" spans="1:38" ht="14.25">
       <c r="A7" s="58" t="s">
         <v>305</v>
       </c>
       <c r="B7" s="58"/>
     </row>
-    <row r="8" spans="1:38">
+    <row r="8" spans="1:38" ht="14.25">
       <c r="A8" s="58" t="s">
         <v>279</v>
       </c>
       <c r="B8" s="58"/>
     </row>
-    <row r="9" spans="1:38">
+    <row r="9" spans="1:38" ht="14.25">
       <c r="B9" s="58" t="s">
         <v>306</v>
       </c>
@@ -22959,7 +22924,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="10" spans="1:38">
+    <row r="10" spans="1:38" ht="14.25">
       <c r="A10" s="58" t="s">
         <v>168</v>
       </c>
@@ -23072,7 +23037,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:38">
+    <row r="11" spans="1:38" ht="14.25">
       <c r="A11" s="58" t="s">
         <v>169</v>
       </c>
@@ -23081,7 +23046,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="12" spans="1:38">
+    <row r="12" spans="1:38" ht="14.25">
       <c r="A12" s="58" t="s">
         <v>308</v>
       </c>
@@ -23194,7 +23159,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:38">
+    <row r="13" spans="1:38" ht="14.25">
       <c r="A13" s="58" t="s">
         <v>310</v>
       </c>
@@ -23307,7 +23272,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:38">
+    <row r="14" spans="1:38" ht="14.25">
       <c r="A14" s="58" t="s">
         <v>312</v>
       </c>
@@ -23420,7 +23385,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:38">
+    <row r="15" spans="1:38" ht="14.25">
       <c r="A15" s="58" t="s">
         <v>170</v>
       </c>
@@ -23429,7 +23394,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="16" spans="1:38">
+    <row r="16" spans="1:38" ht="14.25">
       <c r="A16" s="58" t="s">
         <v>314</v>
       </c>
@@ -23542,7 +23507,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:37" ht="14.25">
       <c r="A17" s="58" t="s">
         <v>316</v>
       </c>
@@ -23655,7 +23620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:37" ht="14.25">
       <c r="A18" s="58" t="s">
         <v>171</v>
       </c>
@@ -23664,7 +23629,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:37" ht="14.25">
       <c r="A19" s="58" t="s">
         <v>318</v>
       </c>
@@ -23673,7 +23638,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:37" ht="14.25">
       <c r="A20" s="58" t="s">
         <v>319</v>
       </c>
@@ -23786,7 +23751,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:37">
+    <row r="21" spans="1:37" ht="14.25">
       <c r="A21" s="58" t="s">
         <v>321</v>
       </c>
@@ -23899,7 +23864,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:37">
+    <row r="22" spans="1:37" ht="14.25">
       <c r="A22" s="58" t="s">
         <v>323</v>
       </c>
@@ -24012,7 +23977,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:37">
+    <row r="23" spans="1:37" ht="14.25">
       <c r="A23" s="58" t="s">
         <v>325</v>
       </c>
@@ -24125,7 +24090,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:37">
+    <row r="24" spans="1:37" ht="14.25">
       <c r="A24" s="58" t="s">
         <v>327</v>
       </c>
@@ -24238,7 +24203,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:37">
+    <row r="25" spans="1:37" ht="14.25">
       <c r="A25" s="58" t="s">
         <v>329</v>
       </c>
@@ -24351,7 +24316,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="26" spans="1:37">
+    <row r="26" spans="1:37" ht="14.25">
       <c r="A26" s="58" t="s">
         <v>331</v>
       </c>
@@ -24464,7 +24429,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="27" spans="1:37">
+    <row r="27" spans="1:37" ht="14.25">
       <c r="A27" s="58" t="s">
         <v>333</v>
       </c>
@@ -24577,7 +24542,7 @@
         <v>-2E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:37">
+    <row r="28" spans="1:37" ht="14.25">
       <c r="A28" s="58" t="s">
         <v>335</v>
       </c>
@@ -24690,7 +24655,7 @@
         <v>-1E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:37">
+    <row r="29" spans="1:37" ht="14.25">
       <c r="A29" s="58" t="s">
         <v>337</v>
       </c>
@@ -24803,7 +24768,7 @@
         <v>-4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:37">
+    <row r="30" spans="1:37" ht="14.25">
       <c r="A30" s="58" t="s">
         <v>339</v>
       </c>
@@ -24916,7 +24881,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:37">
+    <row r="31" spans="1:37" ht="14.25">
       <c r="A31" s="58" t="s">
         <v>341</v>
       </c>
@@ -25029,7 +24994,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:37">
+    <row r="32" spans="1:37" ht="14.25">
       <c r="A32" s="58" t="s">
         <v>343</v>
       </c>
@@ -25142,7 +25107,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="33" spans="1:37">
+    <row r="33" spans="1:37" ht="14.25">
       <c r="A33" s="58" t="s">
         <v>172</v>
       </c>
@@ -25151,7 +25116,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="34" spans="1:37">
+    <row r="34" spans="1:37" ht="14.25">
       <c r="A34" s="58" t="s">
         <v>345</v>
       </c>
@@ -25160,7 +25125,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="35" spans="1:37">
+    <row r="35" spans="1:37" ht="14.25">
       <c r="A35" s="58" t="s">
         <v>308</v>
       </c>
@@ -25169,7 +25134,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="36" spans="1:37">
+    <row r="36" spans="1:37" ht="14.25">
       <c r="A36" s="58" t="s">
         <v>319</v>
       </c>
@@ -25282,7 +25247,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:37">
+    <row r="37" spans="1:37" ht="14.25">
       <c r="A37" s="58" t="s">
         <v>321</v>
       </c>
@@ -25395,7 +25360,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:37">
+    <row r="38" spans="1:37" ht="14.25">
       <c r="A38" s="58" t="s">
         <v>323</v>
       </c>
@@ -25508,7 +25473,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:37">
+    <row r="39" spans="1:37" ht="14.25">
       <c r="A39" s="58" t="s">
         <v>325</v>
       </c>
@@ -25621,7 +25586,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:37">
+    <row r="40" spans="1:37" ht="14.25">
       <c r="A40" s="58" t="s">
         <v>327</v>
       </c>
@@ -25734,7 +25699,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="41" spans="1:37">
+    <row r="41" spans="1:37" ht="14.25">
       <c r="A41" s="58" t="s">
         <v>329</v>
       </c>
@@ -25847,7 +25812,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:37">
+    <row r="42" spans="1:37" ht="14.25">
       <c r="A42" s="58" t="s">
         <v>331</v>
       </c>
@@ -25960,7 +25925,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:37">
+    <row r="43" spans="1:37" ht="14.25">
       <c r="A43" s="58" t="s">
         <v>333</v>
       </c>
@@ -26073,7 +26038,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:37">
+    <row r="44" spans="1:37" ht="14.25">
       <c r="A44" s="58" t="s">
         <v>335</v>
       </c>
@@ -26186,7 +26151,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:37">
+    <row r="45" spans="1:37" ht="14.25">
       <c r="A45" s="58" t="s">
         <v>337</v>
       </c>
@@ -26299,7 +26264,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="46" spans="1:37">
+    <row r="46" spans="1:37" ht="14.25">
       <c r="A46" s="58" t="s">
         <v>339</v>
       </c>
@@ -26412,7 +26377,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="47" spans="1:37">
+    <row r="47" spans="1:37" ht="14.25">
       <c r="A47" s="58" t="s">
         <v>341</v>
       </c>
@@ -26525,7 +26490,7 @@
         <v>7.2999999999999995E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:37">
+    <row r="48" spans="1:37" ht="14.25">
       <c r="A48" s="58" t="s">
         <v>343</v>
       </c>
@@ -26638,7 +26603,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:37">
+    <row r="49" spans="1:37" ht="14.25">
       <c r="A49" s="58" t="s">
         <v>310</v>
       </c>
@@ -26647,7 +26612,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="50" spans="1:37">
+    <row r="50" spans="1:37" ht="14.25">
       <c r="A50" s="58" t="s">
         <v>319</v>
       </c>
@@ -26760,7 +26725,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:37">
+    <row r="51" spans="1:37" ht="14.25">
       <c r="A51" s="58" t="s">
         <v>321</v>
       </c>
@@ -26873,7 +26838,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:37">
+    <row r="52" spans="1:37" ht="14.25">
       <c r="A52" s="58" t="s">
         <v>323</v>
       </c>
@@ -26986,7 +26951,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:37">
+    <row r="53" spans="1:37" ht="14.25">
       <c r="A53" s="58" t="s">
         <v>325</v>
       </c>
@@ -27099,7 +27064,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:37">
+    <row r="54" spans="1:37" ht="14.25">
       <c r="A54" s="58" t="s">
         <v>327</v>
       </c>
@@ -27212,7 +27177,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:37">
+    <row r="55" spans="1:37" ht="14.25">
       <c r="A55" s="58" t="s">
         <v>329</v>
       </c>
@@ -27325,7 +27290,7 @@
         <v>4.3999999999999997E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:37">
+    <row r="56" spans="1:37" ht="14.25">
       <c r="A56" s="58" t="s">
         <v>331</v>
       </c>
@@ -27438,7 +27403,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:37">
+    <row r="57" spans="1:37" ht="14.25">
       <c r="A57" s="58" t="s">
         <v>333</v>
       </c>
@@ -27551,7 +27516,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:37">
+    <row r="58" spans="1:37" ht="14.25">
       <c r="A58" s="58" t="s">
         <v>335</v>
       </c>
@@ -27664,7 +27629,7 @@
         <v>4.3999999999999997E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:37">
+    <row r="59" spans="1:37" ht="14.25">
       <c r="A59" s="58" t="s">
         <v>337</v>
       </c>
@@ -27777,7 +27742,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:37">
+    <row r="60" spans="1:37" ht="14.25">
       <c r="A60" s="58" t="s">
         <v>339</v>
       </c>
@@ -27890,7 +27855,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:37">
+    <row r="61" spans="1:37" ht="14.25">
       <c r="A61" s="58" t="s">
         <v>341</v>
       </c>
@@ -28003,7 +27968,7 @@
         <v>5.5E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:37">
+    <row r="62" spans="1:37" ht="14.25">
       <c r="A62" s="58" t="s">
         <v>343</v>
       </c>
@@ -28116,7 +28081,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:37">
+    <row r="63" spans="1:37" ht="14.25">
       <c r="A63" s="58" t="s">
         <v>372</v>
       </c>
@@ -28125,7 +28090,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="64" spans="1:37">
+    <row r="64" spans="1:37" ht="14.25">
       <c r="A64" s="58" t="s">
         <v>319</v>
       </c>
@@ -28238,7 +28203,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:37">
+    <row r="65" spans="1:37" ht="14.25">
       <c r="A65" s="58" t="s">
         <v>321</v>
       </c>
@@ -28351,7 +28316,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:37">
+    <row r="66" spans="1:37" ht="14.25">
       <c r="A66" s="58" t="s">
         <v>323</v>
       </c>
@@ -28464,7 +28429,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:37">
+    <row r="67" spans="1:37" ht="14.25">
       <c r="A67" s="58" t="s">
         <v>325</v>
       </c>
@@ -28577,7 +28542,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="68" spans="1:37">
+    <row r="68" spans="1:37" ht="14.25">
       <c r="A68" s="58" t="s">
         <v>327</v>
       </c>
@@ -28690,7 +28655,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:37">
+    <row r="69" spans="1:37" ht="14.25">
       <c r="A69" s="58" t="s">
         <v>329</v>
       </c>
@@ -28803,7 +28768,7 @@
         <v>3.9E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:37">
+    <row r="70" spans="1:37" ht="14.25">
       <c r="A70" s="58" t="s">
         <v>331</v>
       </c>
@@ -28916,7 +28881,7 @@
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:37">
+    <row r="71" spans="1:37" ht="14.25">
       <c r="A71" s="58" t="s">
         <v>333</v>
       </c>
@@ -29029,7 +28994,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:37">
+    <row r="72" spans="1:37" ht="14.25">
       <c r="A72" s="58" t="s">
         <v>335</v>
       </c>
@@ -29142,7 +29107,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:37">
+    <row r="73" spans="1:37" ht="14.25">
       <c r="A73" s="58" t="s">
         <v>337</v>
       </c>
@@ -29255,7 +29220,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:37">
+    <row r="74" spans="1:37" ht="14.25">
       <c r="A74" s="58" t="s">
         <v>339</v>
       </c>
@@ -29368,7 +29333,7 @@
         <v>3.9E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:37">
+    <row r="75" spans="1:37" ht="14.25">
       <c r="A75" s="58" t="s">
         <v>341</v>
       </c>
@@ -29481,7 +29446,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:37">
+    <row r="76" spans="1:37" ht="14.25">
       <c r="A76" s="58" t="s">
         <v>343</v>
       </c>
@@ -29594,7 +29559,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:37">
+    <row r="77" spans="1:37" ht="14.25">
       <c r="A77" s="58" t="s">
         <v>175</v>
       </c>
@@ -29707,7 +29672,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:37">
+    <row r="78" spans="1:37" ht="14.25">
       <c r="A78" s="58" t="s">
         <v>173</v>
       </c>
@@ -29716,7 +29681,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="79" spans="1:37">
+    <row r="79" spans="1:37" ht="14.25">
       <c r="A79" s="58" t="s">
         <v>319</v>
       </c>
@@ -29829,7 +29794,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:37">
+    <row r="80" spans="1:37" ht="14.25">
       <c r="A80" s="58" t="s">
         <v>388</v>
       </c>
@@ -29942,7 +29907,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:37">
+    <row r="81" spans="1:37" ht="14.25">
       <c r="A81" s="58" t="s">
         <v>390</v>
       </c>
@@ -30055,7 +30020,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:37">
+    <row r="82" spans="1:37" ht="14.25">
       <c r="A82" s="58" t="s">
         <v>392</v>
       </c>
@@ -30168,7 +30133,7 @@
         <v>-7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:37">
+    <row r="83" spans="1:37" ht="14.25">
       <c r="A83" s="58" t="s">
         <v>321</v>
       </c>
@@ -30281,7 +30246,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:37">
+    <row r="84" spans="1:37" ht="14.25">
       <c r="A84" s="58" t="s">
         <v>323</v>
       </c>
@@ -30394,7 +30359,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:37">
+    <row r="85" spans="1:37" ht="14.25">
       <c r="A85" s="58" t="s">
         <v>325</v>
       </c>
@@ -30507,7 +30472,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:37">
+    <row r="86" spans="1:37" ht="14.25">
       <c r="A86" s="58" t="s">
         <v>327</v>
       </c>
@@ -30620,7 +30585,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:37">
+    <row r="87" spans="1:37" ht="14.25">
       <c r="A87" s="58" t="s">
         <v>329</v>
       </c>
@@ -30733,7 +30698,7 @@
         <v>4.3999999999999997E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:37">
+    <row r="88" spans="1:37" ht="14.25">
       <c r="A88" s="58" t="s">
         <v>331</v>
       </c>
@@ -30846,7 +30811,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:37">
+    <row r="89" spans="1:37" ht="14.25">
       <c r="A89" s="58" t="s">
         <v>333</v>
       </c>
@@ -30959,7 +30924,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:37">
+    <row r="90" spans="1:37" ht="14.25">
       <c r="A90" s="58" t="s">
         <v>335</v>
       </c>
@@ -31072,7 +31037,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:37">
+    <row r="91" spans="1:37" ht="14.25">
       <c r="A91" s="58" t="s">
         <v>337</v>
       </c>
@@ -31185,7 +31150,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:37">
+    <row r="92" spans="1:37" ht="14.25">
       <c r="A92" s="58" t="s">
         <v>339</v>
       </c>
@@ -31298,7 +31263,7 @@
         <v>5.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:37">
+    <row r="93" spans="1:37" ht="14.25">
       <c r="A93" s="58" t="s">
         <v>341</v>
       </c>
@@ -31411,7 +31376,7 @@
         <v>6.2E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:37">
+    <row r="94" spans="1:37" ht="14.25">
       <c r="A94" s="58" t="s">
         <v>343</v>
       </c>
@@ -31524,7 +31489,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:37">
+    <row r="95" spans="1:37" ht="14.25">
       <c r="A95" s="58" t="s">
         <v>175</v>
       </c>
@@ -31637,7 +31602,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:37">
+    <row r="96" spans="1:37" ht="14.25">
       <c r="A96" s="58" t="s">
         <v>174</v>
       </c>
@@ -31646,7 +31611,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="97" spans="1:37">
+    <row r="97" spans="1:37" ht="14.25">
       <c r="A97" s="58" t="s">
         <v>319</v>
       </c>
@@ -31759,7 +31724,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="98" spans="1:37">
+    <row r="98" spans="1:37" ht="14.25">
       <c r="A98" s="58" t="s">
         <v>388</v>
       </c>
@@ -31872,7 +31837,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="99" spans="1:37">
+    <row r="99" spans="1:37" ht="14.25">
       <c r="A99" s="58" t="s">
         <v>390</v>
       </c>
@@ -31985,7 +31950,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:37">
+    <row r="100" spans="1:37" ht="14.25">
       <c r="A100" s="58" t="s">
         <v>392</v>
       </c>
@@ -32098,7 +32063,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="101" spans="1:37">
+    <row r="101" spans="1:37" ht="14.25">
       <c r="A101" s="58" t="s">
         <v>321</v>
       </c>
@@ -32211,7 +32176,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:37">
+    <row r="102" spans="1:37" ht="14.25">
       <c r="A102" s="58" t="s">
         <v>388</v>
       </c>
@@ -32324,7 +32289,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:37">
+    <row r="103" spans="1:37" ht="14.25">
       <c r="A103" s="58" t="s">
         <v>390</v>
       </c>
@@ -32437,7 +32402,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:37">
+    <row r="104" spans="1:37" ht="14.25">
       <c r="A104" s="58" t="s">
         <v>392</v>
       </c>
@@ -32550,7 +32515,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:37">
+    <row r="105" spans="1:37" ht="14.25">
       <c r="A105" s="58" t="s">
         <v>323</v>
       </c>
@@ -32663,7 +32628,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:37">
+    <row r="106" spans="1:37" ht="14.25">
       <c r="A106" s="58" t="s">
         <v>388</v>
       </c>
@@ -32776,7 +32741,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:37">
+    <row r="107" spans="1:37" ht="14.25">
       <c r="A107" s="58" t="s">
         <v>390</v>
       </c>
@@ -32889,7 +32854,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:37">
+    <row r="108" spans="1:37" ht="14.25">
       <c r="A108" s="58" t="s">
         <v>392</v>
       </c>
@@ -33002,7 +32967,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:37">
+    <row r="109" spans="1:37" ht="14.25">
       <c r="A109" s="58" t="s">
         <v>325</v>
       </c>
@@ -33115,7 +33080,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="110" spans="1:37">
+    <row r="110" spans="1:37" ht="14.25">
       <c r="A110" s="58" t="s">
         <v>388</v>
       </c>
@@ -33228,7 +33193,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="111" spans="1:37">
+    <row r="111" spans="1:37" ht="14.25">
       <c r="A111" s="58" t="s">
         <v>390</v>
       </c>
@@ -33341,7 +33306,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="112" spans="1:37">
+    <row r="112" spans="1:37" ht="14.25">
       <c r="A112" s="58" t="s">
         <v>392</v>
       </c>
@@ -33454,7 +33419,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="113" spans="1:37">
+    <row r="113" spans="1:37" ht="14.25">
       <c r="A113" s="58" t="s">
         <v>327</v>
       </c>
@@ -33567,7 +33532,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:37">
+    <row r="114" spans="1:37" ht="14.25">
       <c r="A114" s="58" t="s">
         <v>388</v>
       </c>
@@ -33680,7 +33645,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:37">
+    <row r="115" spans="1:37" ht="14.25">
       <c r="A115" s="58" t="s">
         <v>390</v>
       </c>
@@ -33793,7 +33758,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:37">
+    <row r="116" spans="1:37" ht="14.25">
       <c r="A116" s="58" t="s">
         <v>392</v>
       </c>
@@ -33906,7 +33871,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:37">
+    <row r="117" spans="1:37" ht="14.25">
       <c r="A117" s="58" t="s">
         <v>329</v>
       </c>
@@ -34019,7 +33984,7 @@
         <v>3.9E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:37">
+    <row r="118" spans="1:37" ht="14.25">
       <c r="A118" s="58" t="s">
         <v>388</v>
       </c>
@@ -34132,7 +34097,7 @@
         <v>3.9E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:37">
+    <row r="119" spans="1:37" ht="14.25">
       <c r="A119" s="58" t="s">
         <v>390</v>
       </c>
@@ -34245,7 +34210,7 @@
         <v>3.9E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:37">
+    <row r="120" spans="1:37" ht="14.25">
       <c r="A120" s="58" t="s">
         <v>392</v>
       </c>
@@ -34358,7 +34323,7 @@
         <v>3.9E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:37">
+    <row r="121" spans="1:37" ht="14.25">
       <c r="A121" s="58" t="s">
         <v>331</v>
       </c>
@@ -34471,7 +34436,7 @@
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:37">
+    <row r="122" spans="1:37" ht="14.25">
       <c r="A122" s="58" t="s">
         <v>388</v>
       </c>
@@ -34584,7 +34549,7 @@
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:37">
+    <row r="123" spans="1:37" ht="14.25">
       <c r="A123" s="58" t="s">
         <v>390</v>
       </c>
@@ -34697,7 +34662,7 @@
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:37">
+    <row r="124" spans="1:37" ht="14.25">
       <c r="A124" s="58" t="s">
         <v>392</v>
       </c>
@@ -34810,7 +34775,7 @@
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:37">
+    <row r="125" spans="1:37" ht="14.25">
       <c r="A125" s="58" t="s">
         <v>333</v>
       </c>
@@ -34923,7 +34888,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:37">
+    <row r="126" spans="1:37" ht="14.25">
       <c r="A126" s="58" t="s">
         <v>388</v>
       </c>
@@ -35036,7 +35001,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:37">
+    <row r="127" spans="1:37" ht="14.25">
       <c r="A127" s="58" t="s">
         <v>390</v>
       </c>
@@ -35149,7 +35114,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:37">
+    <row r="128" spans="1:37" ht="14.25">
       <c r="A128" s="58" t="s">
         <v>392</v>
       </c>
@@ -35262,7 +35227,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:37">
+    <row r="129" spans="1:37" ht="14.25">
       <c r="A129" s="58" t="s">
         <v>335</v>
       </c>
@@ -35375,7 +35340,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:37">
+    <row r="130" spans="1:37" ht="14.25">
       <c r="A130" s="58" t="s">
         <v>388</v>
       </c>
@@ -35488,7 +35453,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:37">
+    <row r="131" spans="1:37" ht="14.25">
       <c r="A131" s="58" t="s">
         <v>390</v>
       </c>
@@ -35601,7 +35566,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:37">
+    <row r="132" spans="1:37" ht="14.25">
       <c r="A132" s="58" t="s">
         <v>392</v>
       </c>
@@ -35714,7 +35679,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:37">
+    <row r="133" spans="1:37" ht="14.25">
       <c r="A133" s="58" t="s">
         <v>337</v>
       </c>
@@ -35827,7 +35792,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="134" spans="1:37">
+    <row r="134" spans="1:37" ht="14.25">
       <c r="A134" s="58" t="s">
         <v>388</v>
       </c>
@@ -35940,7 +35905,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="135" spans="1:37">
+    <row r="135" spans="1:37" ht="14.25">
       <c r="A135" s="58" t="s">
         <v>390</v>
       </c>
@@ -36053,7 +36018,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="136" spans="1:37">
+    <row r="136" spans="1:37" ht="14.25">
       <c r="A136" s="58" t="s">
         <v>392</v>
       </c>
@@ -36166,7 +36131,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="137" spans="1:37">
+    <row r="137" spans="1:37" ht="14.25">
       <c r="A137" s="58" t="s">
         <v>339</v>
       </c>
@@ -36279,7 +36244,7 @@
         <v>3.9E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:37">
+    <row r="138" spans="1:37" ht="14.25">
       <c r="A138" s="58" t="s">
         <v>388</v>
       </c>
@@ -36392,7 +36357,7 @@
         <v>3.9E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:37">
+    <row r="139" spans="1:37" ht="14.25">
       <c r="A139" s="58" t="s">
         <v>390</v>
       </c>
@@ -36505,7 +36470,7 @@
         <v>3.9E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:37">
+    <row r="140" spans="1:37" ht="14.25">
       <c r="A140" s="58" t="s">
         <v>392</v>
       </c>
@@ -36618,7 +36583,7 @@
         <v>3.9E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:37">
+    <row r="141" spans="1:37" ht="14.25">
       <c r="A141" s="58" t="s">
         <v>341</v>
       </c>
@@ -36731,7 +36696,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:37">
+    <row r="142" spans="1:37" ht="14.25">
       <c r="A142" s="58" t="s">
         <v>388</v>
       </c>
@@ -36844,7 +36809,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:37">
+    <row r="143" spans="1:37" ht="14.25">
       <c r="A143" s="58" t="s">
         <v>390</v>
       </c>
@@ -36957,7 +36922,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:37">
+    <row r="144" spans="1:37" ht="14.25">
       <c r="A144" s="58" t="s">
         <v>392</v>
       </c>
@@ -37070,7 +37035,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:37">
+    <row r="145" spans="1:37" ht="14.25">
       <c r="A145" s="58" t="s">
         <v>343</v>
       </c>
@@ -37183,7 +37148,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:37">
+    <row r="146" spans="1:37" ht="14.25">
       <c r="A146" s="58" t="s">
         <v>388</v>
       </c>
@@ -37296,7 +37261,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:37">
+    <row r="147" spans="1:37" ht="14.25">
       <c r="A147" s="58" t="s">
         <v>390</v>
       </c>
@@ -37409,7 +37374,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:37">
+    <row r="148" spans="1:37" ht="14.25">
       <c r="A148" s="58" t="s">
         <v>392</v>
       </c>
@@ -37522,7 +37487,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:37">
+    <row r="149" spans="1:37" ht="14.25">
       <c r="A149" s="58" t="s">
         <v>175</v>
       </c>
@@ -37635,7 +37600,7 @@
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:37">
+    <row r="150" spans="1:37" ht="14.25">
       <c r="A150" s="58" t="s">
         <v>176</v>
       </c>
@@ -37644,7 +37609,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="151" spans="1:37">
+    <row r="151" spans="1:37" ht="14.25">
       <c r="A151" s="58" t="s">
         <v>460</v>
       </c>
@@ -37757,7 +37722,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="152" spans="1:37">
+    <row r="152" spans="1:37" ht="14.25">
       <c r="A152" s="58" t="s">
         <v>462</v>
       </c>
@@ -37870,7 +37835,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="153" spans="1:37">
+    <row r="153" spans="1:37" ht="14.25">
       <c r="A153" s="58" t="s">
         <v>464</v>
       </c>
@@ -37983,7 +37948,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="154" spans="1:37">
+    <row r="154" spans="1:37" ht="14.25">
       <c r="A154" s="58" t="s">
         <v>466</v>
       </c>
@@ -38096,7 +38061,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="155" spans="1:37">
+    <row r="155" spans="1:37" ht="14.25">
       <c r="A155" s="58" t="s">
         <v>468</v>
       </c>
@@ -38209,7 +38174,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="156" spans="1:37">
+    <row r="156" spans="1:37" ht="14.25">
       <c r="A156" s="58" t="s">
         <v>470</v>
       </c>
@@ -38322,7 +38287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:37">
+    <row r="157" spans="1:37" ht="14.25">
       <c r="A157" s="58" t="s">
         <v>472</v>
       </c>
@@ -38435,7 +38400,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="158" spans="1:37">
+    <row r="158" spans="1:37" ht="14.25">
       <c r="A158" s="58" t="s">
         <v>474</v>
       </c>
@@ -38548,7 +38513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:37">
+    <row r="159" spans="1:37" ht="14.25">
       <c r="A159" s="58" t="s">
         <v>476</v>
       </c>
@@ -38661,7 +38626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:37">
+    <row r="160" spans="1:37" ht="14.25">
       <c r="A160" s="58" t="s">
         <v>478</v>
       </c>
@@ -38670,7 +38635,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="161" spans="1:37">
+    <row r="161" spans="1:37" ht="14.25">
       <c r="A161" s="58" t="s">
         <v>479</v>
       </c>
@@ -38679,7 +38644,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="162" spans="1:37">
+    <row r="162" spans="1:37" ht="14.25">
       <c r="A162" s="58" t="s">
         <v>388</v>
       </c>
@@ -38792,7 +38757,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="163" spans="1:37">
+    <row r="163" spans="1:37" ht="14.25">
       <c r="A163" s="58" t="s">
         <v>390</v>
       </c>
@@ -38905,7 +38870,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="164" spans="1:37">
+    <row r="164" spans="1:37" ht="14.25">
       <c r="A164" s="58" t="s">
         <v>392</v>
       </c>
@@ -39018,7 +38983,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="165" spans="1:37">
+    <row r="165" spans="1:37" ht="14.25">
       <c r="A165" s="58" t="s">
         <v>483</v>
       </c>
@@ -39131,7 +39096,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="166" spans="1:37">
+    <row r="166" spans="1:37" ht="14.25">
       <c r="A166" s="58" t="s">
         <v>485</v>
       </c>
@@ -39140,7 +39105,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="167" spans="1:37">
+    <row r="167" spans="1:37" ht="14.25">
       <c r="A167" s="58" t="s">
         <v>388</v>
       </c>
@@ -39253,7 +39218,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="168" spans="1:37">
+    <row r="168" spans="1:37" ht="14.25">
       <c r="A168" s="58" t="s">
         <v>390</v>
       </c>
@@ -39366,7 +39331,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="169" spans="1:37">
+    <row r="169" spans="1:37" ht="14.25">
       <c r="A169" s="58" t="s">
         <v>392</v>
       </c>
@@ -39479,7 +39444,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="170" spans="1:37">
+    <row r="170" spans="1:37" ht="14.25">
       <c r="A170" s="58" t="s">
         <v>483</v>
       </c>
@@ -39592,7 +39557,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="171" spans="1:37">
+    <row r="171" spans="1:37" ht="14.25">
       <c r="A171" s="58" t="s">
         <v>178</v>
       </c>
@@ -39601,7 +39566,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="172" spans="1:37">
+    <row r="172" spans="1:37" ht="14.25">
       <c r="A172" s="58" t="s">
         <v>490</v>
       </c>
@@ -39610,7 +39575,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="173" spans="1:37">
+    <row r="173" spans="1:37" ht="14.25">
       <c r="A173" s="58" t="s">
         <v>319</v>
       </c>
@@ -39723,7 +39688,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="174" spans="1:37">
+    <row r="174" spans="1:37" ht="14.25">
       <c r="A174" s="58" t="s">
         <v>321</v>
       </c>
@@ -39836,7 +39801,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:37">
+    <row r="175" spans="1:37" ht="14.25">
       <c r="A175" s="58" t="s">
         <v>323</v>
       </c>
@@ -39949,7 +39914,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:37">
+    <row r="176" spans="1:37" ht="14.25">
       <c r="A176" s="58" t="s">
         <v>325</v>
       </c>
@@ -40062,7 +40027,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="177" spans="1:39">
+    <row r="177" spans="1:39" ht="14.25">
       <c r="A177" s="58" t="s">
         <v>327</v>
       </c>
@@ -40175,7 +40140,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:39">
+    <row r="178" spans="1:39" ht="14.25">
       <c r="A178" s="58" t="s">
         <v>329</v>
       </c>
@@ -40288,7 +40253,7 @@
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:39">
+    <row r="179" spans="1:39" ht="14.25">
       <c r="A179" s="58" t="s">
         <v>331</v>
       </c>
@@ -40401,7 +40366,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="180" spans="1:39">
+    <row r="180" spans="1:39" ht="14.25">
       <c r="A180" s="58" t="s">
         <v>333</v>
       </c>
@@ -40514,7 +40479,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:39">
+    <row r="181" spans="1:39" ht="14.25">
       <c r="A181" s="58" t="s">
         <v>335</v>
       </c>
@@ -40627,7 +40592,7 @@
         <v>3.9E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:39">
+    <row r="182" spans="1:39" ht="14.25">
       <c r="A182" s="58" t="s">
         <v>337</v>
       </c>
@@ -40740,7 +40705,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="183" spans="1:39">
+    <row r="183" spans="1:39" ht="14.25">
       <c r="A183" s="58" t="s">
         <v>339</v>
       </c>
@@ -40853,7 +40818,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:39">
+    <row r="184" spans="1:39" ht="14.25">
       <c r="A184" s="58" t="s">
         <v>341</v>
       </c>
@@ -40966,7 +40931,7 @@
         <v>5.7000000000000002E-2</v>
       </c>
     </row>
-    <row r="185" spans="1:39">
+    <row r="185" spans="1:39" ht="14.25">
       <c r="A185" s="58" t="s">
         <v>343</v>
       </c>
@@ -41079,7 +41044,7 @@
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:39">
+    <row r="186" spans="1:39" ht="14.25">
       <c r="A186" s="58" t="s">
         <v>175</v>
       </c>
@@ -41192,7 +41157,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:39">
+    <row r="187" spans="1:39" ht="14.25">
       <c r="A187" s="58" t="s">
         <v>505</v>
       </c>
@@ -41308,7 +41273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:39">
+    <row r="188" spans="1:39" ht="14.25">
       <c r="A188" s="58" t="s">
         <v>507</v>
       </c>
@@ -41531,11 +41496,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK286"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
@@ -41543,8 +41508,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="45.7109375" customWidth="1"/>
-    <col min="2" max="2" width="69.28515625" customWidth="1"/>
+    <col min="1" max="1" width="45.73046875" customWidth="1"/>
+    <col min="2" max="2" width="69.265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1">
@@ -41814,116 +41779,116 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:37" s="83" customFormat="1" ht="15" customHeight="1">
-      <c r="A10" s="83" t="s">
+    <row r="10" spans="1:37" s="82" customFormat="1" ht="15" customHeight="1">
+      <c r="A10" s="82" t="s">
         <v>709</v>
       </c>
-      <c r="B10" s="83" t="s">
+      <c r="B10" s="82" t="s">
         <v>710</v>
       </c>
-      <c r="C10" s="83" t="s">
+      <c r="C10" s="82" t="s">
         <v>711</v>
       </c>
-      <c r="D10" s="83" t="s">
+      <c r="D10" s="82" t="s">
         <v>298</v>
       </c>
-      <c r="E10" s="83">
+      <c r="E10" s="82">
         <v>12.993387999999999</v>
       </c>
-      <c r="F10" s="83">
+      <c r="F10" s="82">
         <v>13.085564</v>
       </c>
-      <c r="G10" s="83">
+      <c r="G10" s="82">
         <v>13.426015</v>
       </c>
-      <c r="H10" s="83">
+      <c r="H10" s="82">
         <v>13.682649</v>
       </c>
-      <c r="I10" s="83">
+      <c r="I10" s="82">
         <v>13.986616</v>
       </c>
-      <c r="J10" s="83">
+      <c r="J10" s="82">
         <v>14.255686000000001</v>
       </c>
-      <c r="K10" s="83">
+      <c r="K10" s="82">
         <v>14.576639</v>
       </c>
-      <c r="L10" s="83">
+      <c r="L10" s="82">
         <v>14.91924</v>
       </c>
-      <c r="M10" s="83">
+      <c r="M10" s="82">
         <v>15.298795</v>
       </c>
-      <c r="N10" s="83">
+      <c r="N10" s="82">
         <v>15.655293</v>
       </c>
-      <c r="O10" s="83">
+      <c r="O10" s="82">
         <v>16.036183999999999</v>
       </c>
-      <c r="P10" s="83">
+      <c r="P10" s="82">
         <v>16.403683000000001</v>
       </c>
-      <c r="Q10" s="83">
+      <c r="Q10" s="82">
         <v>16.869240000000001</v>
       </c>
-      <c r="R10" s="83">
+      <c r="R10" s="82">
         <v>17.3323</v>
       </c>
-      <c r="S10" s="83">
+      <c r="S10" s="82">
         <v>17.859477999999999</v>
       </c>
-      <c r="T10" s="83">
+      <c r="T10" s="82">
         <v>18.381401</v>
       </c>
-      <c r="U10" s="83">
+      <c r="U10" s="82">
         <v>18.955078</v>
       </c>
-      <c r="V10" s="83">
+      <c r="V10" s="82">
         <v>19.562397000000001</v>
       </c>
-      <c r="W10" s="83">
+      <c r="W10" s="82">
         <v>20.127655000000001</v>
       </c>
-      <c r="X10" s="83">
+      <c r="X10" s="82">
         <v>20.680295999999998</v>
       </c>
-      <c r="Y10" s="83">
+      <c r="Y10" s="82">
         <v>21.201677</v>
       </c>
-      <c r="Z10" s="83">
+      <c r="Z10" s="82">
         <v>21.717047000000001</v>
       </c>
-      <c r="AA10" s="83">
+      <c r="AA10" s="82">
         <v>22.233829</v>
       </c>
-      <c r="AB10" s="83">
+      <c r="AB10" s="82">
         <v>22.74757</v>
       </c>
-      <c r="AC10" s="83">
+      <c r="AC10" s="82">
         <v>23.234901000000001</v>
       </c>
-      <c r="AD10" s="83">
+      <c r="AD10" s="82">
         <v>23.752506</v>
       </c>
-      <c r="AE10" s="83">
+      <c r="AE10" s="82">
         <v>24.289179000000001</v>
       </c>
-      <c r="AF10" s="83">
+      <c r="AF10" s="82">
         <v>24.883963000000001</v>
       </c>
-      <c r="AG10" s="83">
+      <c r="AG10" s="82">
         <v>25.396719000000001</v>
       </c>
-      <c r="AH10" s="83">
+      <c r="AH10" s="82">
         <v>25.982728999999999</v>
       </c>
-      <c r="AI10" s="83">
+      <c r="AI10" s="82">
         <v>26.591958999999999</v>
       </c>
-      <c r="AJ10" s="83">
+      <c r="AJ10" s="82">
         <v>27.240181</v>
       </c>
-      <c r="AK10" s="84">
+      <c r="AK10" s="83">
         <v>2.4E-2</v>
       </c>
     </row>
@@ -42952,116 +42917,116 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:37" s="83" customFormat="1" ht="15" customHeight="1">
-      <c r="A21" s="83" t="s">
+    <row r="21" spans="1:37" s="82" customFormat="1" ht="15" customHeight="1">
+      <c r="A21" s="82" t="s">
         <v>709</v>
       </c>
-      <c r="B21" s="83" t="s">
+      <c r="B21" s="82" t="s">
         <v>740</v>
       </c>
-      <c r="C21" s="83" t="s">
+      <c r="C21" s="82" t="s">
         <v>741</v>
       </c>
-      <c r="D21" s="83" t="s">
+      <c r="D21" s="82" t="s">
         <v>298</v>
       </c>
-      <c r="E21" s="83">
+      <c r="E21" s="82">
         <v>16.566603000000001</v>
       </c>
-      <c r="F21" s="83">
+      <c r="F21" s="82">
         <v>16.396280000000001</v>
       </c>
-      <c r="G21" s="83">
+      <c r="G21" s="82">
         <v>16.439896000000001</v>
       </c>
-      <c r="H21" s="83">
+      <c r="H21" s="82">
         <v>16.529689999999999</v>
       </c>
-      <c r="I21" s="83">
+      <c r="I21" s="82">
         <v>16.688790999999998</v>
       </c>
-      <c r="J21" s="83">
+      <c r="J21" s="82">
         <v>16.827316</v>
       </c>
-      <c r="K21" s="83">
+      <c r="K21" s="82">
         <v>17.001038000000001</v>
       </c>
-      <c r="L21" s="83">
+      <c r="L21" s="82">
         <v>17.231853000000001</v>
       </c>
-      <c r="M21" s="83">
+      <c r="M21" s="82">
         <v>17.535267000000001</v>
       </c>
-      <c r="N21" s="83">
+      <c r="N21" s="82">
         <v>17.869351999999999</v>
       </c>
-      <c r="O21" s="83">
+      <c r="O21" s="82">
         <v>18.247271000000001</v>
       </c>
-      <c r="P21" s="83">
+      <c r="P21" s="82">
         <v>18.587626</v>
       </c>
-      <c r="Q21" s="83">
+      <c r="Q21" s="82">
         <v>19.025107999999999</v>
       </c>
-      <c r="R21" s="83">
+      <c r="R21" s="82">
         <v>19.452936000000001</v>
       </c>
-      <c r="S21" s="83">
+      <c r="S21" s="82">
         <v>19.913948000000001</v>
       </c>
-      <c r="T21" s="83">
+      <c r="T21" s="82">
         <v>20.349620999999999</v>
       </c>
-      <c r="U21" s="83">
+      <c r="U21" s="82">
         <v>20.815242999999999</v>
       </c>
-      <c r="V21" s="83">
+      <c r="V21" s="82">
         <v>21.332705000000001</v>
       </c>
-      <c r="W21" s="83">
+      <c r="W21" s="82">
         <v>21.817457000000001</v>
       </c>
-      <c r="X21" s="83">
+      <c r="X21" s="82">
         <v>22.307468</v>
       </c>
-      <c r="Y21" s="83">
+      <c r="Y21" s="82">
         <v>22.81044</v>
       </c>
-      <c r="Z21" s="83">
+      <c r="Z21" s="82">
         <v>23.333673000000001</v>
       </c>
-      <c r="AA21" s="83">
+      <c r="AA21" s="82">
         <v>23.874891000000002</v>
       </c>
-      <c r="AB21" s="83">
+      <c r="AB21" s="82">
         <v>24.436152</v>
       </c>
-      <c r="AC21" s="83">
+      <c r="AC21" s="82">
         <v>25.008697999999999</v>
       </c>
-      <c r="AD21" s="83">
+      <c r="AD21" s="82">
         <v>25.639744</v>
       </c>
-      <c r="AE21" s="83">
+      <c r="AE21" s="82">
         <v>26.300379</v>
       </c>
-      <c r="AF21" s="83">
+      <c r="AF21" s="82">
         <v>27.032423000000001</v>
       </c>
-      <c r="AG21" s="83">
+      <c r="AG21" s="82">
         <v>27.666231</v>
       </c>
-      <c r="AH21" s="83">
+      <c r="AH21" s="82">
         <v>28.366410999999999</v>
       </c>
-      <c r="AI21" s="83">
+      <c r="AI21" s="82">
         <v>29.091557999999999</v>
       </c>
-      <c r="AJ21" s="83">
+      <c r="AJ21" s="82">
         <v>29.820221</v>
       </c>
-      <c r="AK21" s="84">
+      <c r="AK21" s="83">
         <v>1.9E-2</v>
       </c>
     </row>
@@ -44090,116 +44055,116 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:37" s="83" customFormat="1" ht="15" customHeight="1">
-      <c r="A32" s="83" t="s">
+    <row r="32" spans="1:37" s="82" customFormat="1" ht="15" customHeight="1">
+      <c r="A32" s="82" t="s">
         <v>709</v>
       </c>
-      <c r="B32" s="83" t="s">
+      <c r="B32" s="82" t="s">
         <v>763</v>
       </c>
-      <c r="C32" s="83" t="s">
+      <c r="C32" s="82" t="s">
         <v>764</v>
       </c>
-      <c r="D32" s="83" t="s">
+      <c r="D32" s="82" t="s">
         <v>298</v>
       </c>
-      <c r="E32" s="83">
+      <c r="E32" s="82">
         <v>0.18604699999999999</v>
       </c>
-      <c r="F32" s="83">
+      <c r="F32" s="82">
         <v>0.164021</v>
       </c>
-      <c r="G32" s="83">
+      <c r="G32" s="82">
         <v>0.147254</v>
       </c>
-      <c r="H32" s="83">
+      <c r="H32" s="82">
         <v>0.13270699999999999</v>
       </c>
-      <c r="I32" s="83">
+      <c r="I32" s="82">
         <v>0.121167</v>
       </c>
-      <c r="J32" s="83">
+      <c r="J32" s="82">
         <v>0.111348</v>
       </c>
-      <c r="K32" s="83">
+      <c r="K32" s="82">
         <v>0.10306899999999999</v>
       </c>
-      <c r="L32" s="83">
+      <c r="L32" s="82">
         <v>9.6655000000000005E-2</v>
       </c>
-      <c r="M32" s="83">
+      <c r="M32" s="82">
         <v>9.1883999999999993E-2</v>
       </c>
-      <c r="N32" s="83">
+      <c r="N32" s="82">
         <v>8.7783E-2</v>
       </c>
-      <c r="O32" s="83">
+      <c r="O32" s="82">
         <v>8.4326999999999999E-2</v>
       </c>
-      <c r="P32" s="83">
+      <c r="P32" s="82">
         <v>8.1729999999999997E-2</v>
       </c>
-      <c r="Q32" s="83">
+      <c r="Q32" s="82">
         <v>7.9777000000000001E-2</v>
       </c>
-      <c r="R32" s="83">
+      <c r="R32" s="82">
         <v>7.7663999999999997E-2</v>
       </c>
-      <c r="S32" s="83">
+      <c r="S32" s="82">
         <v>7.6067999999999997E-2</v>
       </c>
-      <c r="T32" s="83">
+      <c r="T32" s="82">
         <v>7.4709999999999999E-2</v>
       </c>
-      <c r="U32" s="83">
+      <c r="U32" s="82">
         <v>7.3875999999999997E-2</v>
       </c>
-      <c r="V32" s="83">
+      <c r="V32" s="82">
         <v>7.3050000000000004E-2</v>
       </c>
-      <c r="W32" s="83">
+      <c r="W32" s="82">
         <v>7.2313000000000002E-2</v>
       </c>
-      <c r="X32" s="83">
+      <c r="X32" s="82">
         <v>7.1783E-2</v>
       </c>
-      <c r="Y32" s="83">
+      <c r="Y32" s="82">
         <v>7.1441000000000004E-2</v>
       </c>
-      <c r="Z32" s="83">
+      <c r="Z32" s="82">
         <v>7.1091000000000001E-2</v>
       </c>
-      <c r="AA32" s="83">
+      <c r="AA32" s="82">
         <v>7.0878999999999998E-2</v>
       </c>
-      <c r="AB32" s="83">
+      <c r="AB32" s="82">
         <v>7.0614999999999997E-2</v>
       </c>
-      <c r="AC32" s="83">
+      <c r="AC32" s="82">
         <v>7.0347999999999994E-2</v>
       </c>
-      <c r="AD32" s="83">
+      <c r="AD32" s="82">
         <v>7.0442000000000005E-2</v>
       </c>
-      <c r="AE32" s="83">
+      <c r="AE32" s="82">
         <v>7.0763000000000006E-2</v>
       </c>
-      <c r="AF32" s="83">
+      <c r="AF32" s="82">
         <v>7.1356000000000003E-2</v>
       </c>
-      <c r="AG32" s="83">
+      <c r="AG32" s="82">
         <v>7.1734000000000006E-2</v>
       </c>
-      <c r="AH32" s="83">
+      <c r="AH32" s="82">
         <v>7.2326000000000001E-2</v>
       </c>
-      <c r="AI32" s="83">
+      <c r="AI32" s="82">
         <v>7.2960999999999998E-2</v>
       </c>
-      <c r="AJ32" s="83">
+      <c r="AJ32" s="82">
         <v>7.3634000000000005E-2</v>
       </c>
-      <c r="AK32" s="84">
+      <c r="AK32" s="83">
         <v>-2.9000000000000001E-2</v>
       </c>
     </row>

</xml_diff>